<commit_message>
add param min_sample_N in plot.pro_bar_data
</commit_message>
<xml_diff>
--- a/data/plot.xlsx
+++ b/data/plot.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_Progs\BA\Python\BA_PY\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB6C60-5DA4-4C31-AE54-A55A9A13A9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C038BA0-57D8-4624-80B0-1C5CCB49B5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1752" yWindow="1944" windowWidth="17280" windowHeight="10320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="xm" sheetId="1" r:id="rId1"/>
     <sheet name="ym" sheetId="2" r:id="rId2"/>
     <sheet name="peak" sheetId="3" r:id="rId3"/>
+    <sheet name="weight" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="40">
   <si>
     <t>solution</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,6 +162,24 @@
   </si>
   <si>
     <t>CaCl</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>Exp</t>
   </si>
 </sst>
 </file>
@@ -2874,7 +2893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8414DC0A-3BFB-4F56-82E3-648AE5F250A1}">
   <dimension ref="A1:E289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -7794,4 +7813,4896 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579F8FC8-BF69-49E4-886E-5CD872A47A8A}">
+  <dimension ref="A1:E287"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>360</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>360</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>362</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>372</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>374</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>385</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>384</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>392</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>390</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>405</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>414</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>416</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>350</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>350</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>353</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>360</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>364</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>380</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>385</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>391</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>394</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>411</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>420</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>429</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>392</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>392</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>387</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>403</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>422</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>424</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>435</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>452</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>462</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>17</v>
+      </c>
+      <c r="C35">
+        <v>480</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <v>488</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>21</v>
+      </c>
+      <c r="C37">
+        <v>495</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>376</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>376</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>348</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>356</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>370</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>360</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>380</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>390</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="C46">
+        <v>393</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>17</v>
+      </c>
+      <c r="C47">
+        <v>398</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>19</v>
+      </c>
+      <c r="C48">
+        <v>396</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>21</v>
+      </c>
+      <c r="C49">
+        <v>399</v>
+      </c>
+      <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>395</v>
+      </c>
+      <c r="D50">
+        <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>395</v>
+      </c>
+      <c r="D51">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>370</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>328</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>340</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>342</v>
+      </c>
+      <c r="D55">
+        <v>8</v>
+      </c>
+      <c r="E55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>365</v>
+      </c>
+      <c r="D56">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>13</v>
+      </c>
+      <c r="C57">
+        <v>391</v>
+      </c>
+      <c r="D57">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>15</v>
+      </c>
+      <c r="C58">
+        <v>388</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>17</v>
+      </c>
+      <c r="C59">
+        <v>382</v>
+      </c>
+      <c r="D59">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>19</v>
+      </c>
+      <c r="C60">
+        <v>368</v>
+      </c>
+      <c r="D60">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>21</v>
+      </c>
+      <c r="C61">
+        <v>398</v>
+      </c>
+      <c r="D61">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>23</v>
+      </c>
+      <c r="C62">
+        <v>389</v>
+      </c>
+      <c r="D62">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>347</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>347</v>
+      </c>
+      <c r="D64">
+        <v>10</v>
+      </c>
+      <c r="E64" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>325</v>
+      </c>
+      <c r="D65">
+        <v>10</v>
+      </c>
+      <c r="E65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>328</v>
+      </c>
+      <c r="D66">
+        <v>10</v>
+      </c>
+      <c r="E66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>7</v>
+      </c>
+      <c r="C67">
+        <v>330</v>
+      </c>
+      <c r="D67">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <v>330</v>
+      </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>11</v>
+      </c>
+      <c r="C69">
+        <v>330</v>
+      </c>
+      <c r="D69">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>13</v>
+      </c>
+      <c r="C70">
+        <v>346</v>
+      </c>
+      <c r="D70">
+        <v>10</v>
+      </c>
+      <c r="E70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>15</v>
+      </c>
+      <c r="C71">
+        <v>350</v>
+      </c>
+      <c r="D71">
+        <v>10</v>
+      </c>
+      <c r="E71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>17</v>
+      </c>
+      <c r="C72">
+        <v>357</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>19</v>
+      </c>
+      <c r="C73">
+        <v>366</v>
+      </c>
+      <c r="D73">
+        <v>10</v>
+      </c>
+      <c r="E73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>21</v>
+      </c>
+      <c r="C74">
+        <v>368</v>
+      </c>
+      <c r="D74">
+        <v>10</v>
+      </c>
+      <c r="E74" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>23</v>
+      </c>
+      <c r="C75">
+        <v>380</v>
+      </c>
+      <c r="D75">
+        <v>10</v>
+      </c>
+      <c r="E75" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>370</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
+      </c>
+      <c r="E76" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>370</v>
+      </c>
+      <c r="D77">
+        <v>12</v>
+      </c>
+      <c r="E77" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <v>341</v>
+      </c>
+      <c r="D78">
+        <v>12</v>
+      </c>
+      <c r="E78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>365</v>
+      </c>
+      <c r="D79">
+        <v>12</v>
+      </c>
+      <c r="E79" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>7</v>
+      </c>
+      <c r="C80">
+        <v>375</v>
+      </c>
+      <c r="D80">
+        <v>12</v>
+      </c>
+      <c r="E80" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>9</v>
+      </c>
+      <c r="C81">
+        <v>380</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+      <c r="E81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>11</v>
+      </c>
+      <c r="C82">
+        <v>400</v>
+      </c>
+      <c r="D82">
+        <v>12</v>
+      </c>
+      <c r="E82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>13</v>
+      </c>
+      <c r="C83">
+        <v>418</v>
+      </c>
+      <c r="D83">
+        <v>12</v>
+      </c>
+      <c r="E83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>15</v>
+      </c>
+      <c r="C84">
+        <v>425</v>
+      </c>
+      <c r="D84">
+        <v>12</v>
+      </c>
+      <c r="E84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>17</v>
+      </c>
+      <c r="C85">
+        <v>443</v>
+      </c>
+      <c r="D85">
+        <v>12</v>
+      </c>
+      <c r="E85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>19</v>
+      </c>
+      <c r="C86">
+        <v>449</v>
+      </c>
+      <c r="D86">
+        <v>12</v>
+      </c>
+      <c r="E86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>21</v>
+      </c>
+      <c r="C87">
+        <v>453</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>370</v>
+      </c>
+      <c r="D88">
+        <v>14</v>
+      </c>
+      <c r="E88" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>370</v>
+      </c>
+      <c r="D89">
+        <v>14</v>
+      </c>
+      <c r="E89" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>3</v>
+      </c>
+      <c r="C90">
+        <v>367</v>
+      </c>
+      <c r="D90">
+        <v>14</v>
+      </c>
+      <c r="E90" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>5</v>
+      </c>
+      <c r="C91">
+        <v>364</v>
+      </c>
+      <c r="D91">
+        <v>14</v>
+      </c>
+      <c r="E91" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+      <c r="C92">
+        <v>375</v>
+      </c>
+      <c r="D92">
+        <v>14</v>
+      </c>
+      <c r="E92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+      <c r="C93">
+        <v>390</v>
+      </c>
+      <c r="D93">
+        <v>14</v>
+      </c>
+      <c r="E93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <v>412</v>
+      </c>
+      <c r="D94">
+        <v>14</v>
+      </c>
+      <c r="E94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>13</v>
+      </c>
+      <c r="C95">
+        <v>427</v>
+      </c>
+      <c r="D95">
+        <v>14</v>
+      </c>
+      <c r="E95" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>15</v>
+      </c>
+      <c r="C96">
+        <v>430</v>
+      </c>
+      <c r="D96">
+        <v>14</v>
+      </c>
+      <c r="E96" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>17</v>
+      </c>
+      <c r="C97">
+        <v>450</v>
+      </c>
+      <c r="D97">
+        <v>14</v>
+      </c>
+      <c r="E97" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>19</v>
+      </c>
+      <c r="C98">
+        <v>452</v>
+      </c>
+      <c r="D98">
+        <v>14</v>
+      </c>
+      <c r="E98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>21</v>
+      </c>
+      <c r="C99">
+        <v>455</v>
+      </c>
+      <c r="D99">
+        <v>14</v>
+      </c>
+      <c r="E99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>395</v>
+      </c>
+      <c r="D100">
+        <v>16</v>
+      </c>
+      <c r="E100" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>395</v>
+      </c>
+      <c r="D101">
+        <v>16</v>
+      </c>
+      <c r="E101" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+      <c r="C102">
+        <v>385</v>
+      </c>
+      <c r="D102">
+        <v>16</v>
+      </c>
+      <c r="E102" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>380</v>
+      </c>
+      <c r="D103">
+        <v>16</v>
+      </c>
+      <c r="E103" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>7</v>
+      </c>
+      <c r="C104">
+        <v>382</v>
+      </c>
+      <c r="D104">
+        <v>16</v>
+      </c>
+      <c r="E104" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>9</v>
+      </c>
+      <c r="C105">
+        <v>394</v>
+      </c>
+      <c r="D105">
+        <v>16</v>
+      </c>
+      <c r="E105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>11</v>
+      </c>
+      <c r="C106">
+        <v>400</v>
+      </c>
+      <c r="D106">
+        <v>16</v>
+      </c>
+      <c r="E106" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>13</v>
+      </c>
+      <c r="C107">
+        <v>402</v>
+      </c>
+      <c r="D107">
+        <v>16</v>
+      </c>
+      <c r="E107" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>15</v>
+      </c>
+      <c r="C108">
+        <v>402</v>
+      </c>
+      <c r="D108">
+        <v>16</v>
+      </c>
+      <c r="E108" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>17</v>
+      </c>
+      <c r="C109">
+        <v>411</v>
+      </c>
+      <c r="D109">
+        <v>16</v>
+      </c>
+      <c r="E109" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>19</v>
+      </c>
+      <c r="C110">
+        <v>418</v>
+      </c>
+      <c r="D110">
+        <v>16</v>
+      </c>
+      <c r="E110" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>21</v>
+      </c>
+      <c r="C111">
+        <v>416</v>
+      </c>
+      <c r="D111">
+        <v>16</v>
+      </c>
+      <c r="E111" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>420</v>
+      </c>
+      <c r="D112">
+        <v>18</v>
+      </c>
+      <c r="E112" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113">
+        <v>420</v>
+      </c>
+      <c r="D113">
+        <v>18</v>
+      </c>
+      <c r="E113" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>3</v>
+      </c>
+      <c r="C114">
+        <v>418</v>
+      </c>
+      <c r="D114">
+        <v>18</v>
+      </c>
+      <c r="E114" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>5</v>
+      </c>
+      <c r="C115">
+        <v>437</v>
+      </c>
+      <c r="D115">
+        <v>18</v>
+      </c>
+      <c r="E115" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>7</v>
+      </c>
+      <c r="C116">
+        <v>442</v>
+      </c>
+      <c r="D116">
+        <v>18</v>
+      </c>
+      <c r="E116" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>9</v>
+      </c>
+      <c r="C117">
+        <v>447</v>
+      </c>
+      <c r="D117">
+        <v>18</v>
+      </c>
+      <c r="E117" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>11</v>
+      </c>
+      <c r="C118">
+        <v>458</v>
+      </c>
+      <c r="D118">
+        <v>18</v>
+      </c>
+      <c r="E118" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>13</v>
+      </c>
+      <c r="C119">
+        <v>463</v>
+      </c>
+      <c r="D119">
+        <v>18</v>
+      </c>
+      <c r="E119" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>15</v>
+      </c>
+      <c r="C120">
+        <v>471</v>
+      </c>
+      <c r="D120">
+        <v>18</v>
+      </c>
+      <c r="E120" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>17</v>
+      </c>
+      <c r="C121">
+        <v>484</v>
+      </c>
+      <c r="D121">
+        <v>18</v>
+      </c>
+      <c r="E121" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>19</v>
+      </c>
+      <c r="C122">
+        <v>497</v>
+      </c>
+      <c r="D122">
+        <v>18</v>
+      </c>
+      <c r="E122" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>21</v>
+      </c>
+      <c r="C123">
+        <v>490</v>
+      </c>
+      <c r="D123">
+        <v>18</v>
+      </c>
+      <c r="E123" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <v>23</v>
+      </c>
+      <c r="C124">
+        <v>506</v>
+      </c>
+      <c r="D124">
+        <v>18</v>
+      </c>
+      <c r="E124" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>410</v>
+      </c>
+      <c r="D125">
+        <v>20</v>
+      </c>
+      <c r="E125" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="C126">
+        <v>410</v>
+      </c>
+      <c r="D126">
+        <v>20</v>
+      </c>
+      <c r="E126" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>3</v>
+      </c>
+      <c r="C127">
+        <v>373</v>
+      </c>
+      <c r="D127">
+        <v>20</v>
+      </c>
+      <c r="E127" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>5</v>
+      </c>
+      <c r="C128">
+        <v>389</v>
+      </c>
+      <c r="D128">
+        <v>20</v>
+      </c>
+      <c r="E128" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>7</v>
+      </c>
+      <c r="C129">
+        <v>393</v>
+      </c>
+      <c r="D129">
+        <v>20</v>
+      </c>
+      <c r="E129" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>9</v>
+      </c>
+      <c r="C130">
+        <v>410</v>
+      </c>
+      <c r="D130">
+        <v>20</v>
+      </c>
+      <c r="E130" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>11</v>
+      </c>
+      <c r="C131">
+        <v>427</v>
+      </c>
+      <c r="D131">
+        <v>20</v>
+      </c>
+      <c r="E131" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>13</v>
+      </c>
+      <c r="C132">
+        <v>470</v>
+      </c>
+      <c r="D132">
+        <v>20</v>
+      </c>
+      <c r="E132" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>15</v>
+      </c>
+      <c r="C133">
+        <v>435</v>
+      </c>
+      <c r="D133">
+        <v>20</v>
+      </c>
+      <c r="E133" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>17</v>
+      </c>
+      <c r="C134">
+        <v>446</v>
+      </c>
+      <c r="D134">
+        <v>20</v>
+      </c>
+      <c r="E134" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>19</v>
+      </c>
+      <c r="C135">
+        <v>457</v>
+      </c>
+      <c r="D135">
+        <v>20</v>
+      </c>
+      <c r="E135" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>21</v>
+      </c>
+      <c r="C136">
+        <v>449</v>
+      </c>
+      <c r="D136">
+        <v>20</v>
+      </c>
+      <c r="E136" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>23</v>
+      </c>
+      <c r="C137">
+        <v>464</v>
+      </c>
+      <c r="D137">
+        <v>20</v>
+      </c>
+      <c r="E137" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>370</v>
+      </c>
+      <c r="D138">
+        <v>22</v>
+      </c>
+      <c r="E138" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>370</v>
+      </c>
+      <c r="D139">
+        <v>22</v>
+      </c>
+      <c r="E139" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>3</v>
+      </c>
+      <c r="C140">
+        <v>335</v>
+      </c>
+      <c r="D140">
+        <v>22</v>
+      </c>
+      <c r="E140" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>5</v>
+      </c>
+      <c r="C141">
+        <v>270</v>
+      </c>
+      <c r="D141">
+        <v>22</v>
+      </c>
+      <c r="E141" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>7</v>
+      </c>
+      <c r="C142">
+        <v>344</v>
+      </c>
+      <c r="D142">
+        <v>22</v>
+      </c>
+      <c r="E142" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>9</v>
+      </c>
+      <c r="C143">
+        <v>345</v>
+      </c>
+      <c r="D143">
+        <v>22</v>
+      </c>
+      <c r="E143" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>11</v>
+      </c>
+      <c r="C144">
+        <v>351</v>
+      </c>
+      <c r="D144">
+        <v>22</v>
+      </c>
+      <c r="E144" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>13</v>
+      </c>
+      <c r="C145">
+        <v>400</v>
+      </c>
+      <c r="D145">
+        <v>22</v>
+      </c>
+      <c r="E145" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>15</v>
+      </c>
+      <c r="C146">
+        <v>390</v>
+      </c>
+      <c r="D146">
+        <v>22</v>
+      </c>
+      <c r="E146" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>17</v>
+      </c>
+      <c r="C147">
+        <v>412</v>
+      </c>
+      <c r="D147">
+        <v>22</v>
+      </c>
+      <c r="E147" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>19</v>
+      </c>
+      <c r="C148">
+        <v>420</v>
+      </c>
+      <c r="D148">
+        <v>22</v>
+      </c>
+      <c r="E148" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>21</v>
+      </c>
+      <c r="C149">
+        <v>431</v>
+      </c>
+      <c r="D149">
+        <v>22</v>
+      </c>
+      <c r="E149" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>365</v>
+      </c>
+      <c r="D150">
+        <v>24</v>
+      </c>
+      <c r="E150" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>365</v>
+      </c>
+      <c r="D151">
+        <v>24</v>
+      </c>
+      <c r="E151" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <v>3</v>
+      </c>
+      <c r="C152">
+        <v>365</v>
+      </c>
+      <c r="D152">
+        <v>24</v>
+      </c>
+      <c r="E152" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <v>5</v>
+      </c>
+      <c r="C153">
+        <v>390</v>
+      </c>
+      <c r="D153">
+        <v>24</v>
+      </c>
+      <c r="E153" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <v>7</v>
+      </c>
+      <c r="C154">
+        <v>407</v>
+      </c>
+      <c r="D154">
+        <v>24</v>
+      </c>
+      <c r="E154" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>9</v>
+      </c>
+      <c r="C155">
+        <v>423</v>
+      </c>
+      <c r="D155">
+        <v>24</v>
+      </c>
+      <c r="E155" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <v>11</v>
+      </c>
+      <c r="C156">
+        <v>429</v>
+      </c>
+      <c r="D156">
+        <v>24</v>
+      </c>
+      <c r="E156" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>13</v>
+      </c>
+      <c r="C157">
+        <v>443</v>
+      </c>
+      <c r="D157">
+        <v>24</v>
+      </c>
+      <c r="E157" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>15</v>
+      </c>
+      <c r="C158">
+        <v>448</v>
+      </c>
+      <c r="D158">
+        <v>24</v>
+      </c>
+      <c r="E158" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <v>17</v>
+      </c>
+      <c r="C159">
+        <v>453</v>
+      </c>
+      <c r="D159">
+        <v>24</v>
+      </c>
+      <c r="E159" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <v>19</v>
+      </c>
+      <c r="C160">
+        <v>464</v>
+      </c>
+      <c r="D160">
+        <v>24</v>
+      </c>
+      <c r="E160" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <v>21</v>
+      </c>
+      <c r="C161">
+        <v>457</v>
+      </c>
+      <c r="D161">
+        <v>24</v>
+      </c>
+      <c r="E161" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>315</v>
+      </c>
+      <c r="D162">
+        <v>26</v>
+      </c>
+      <c r="E162" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>283</v>
+      </c>
+      <c r="D163">
+        <v>26</v>
+      </c>
+      <c r="E163" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>162</v>
+      </c>
+      <c r="B164">
+        <v>3</v>
+      </c>
+      <c r="C164">
+        <v>268</v>
+      </c>
+      <c r="D164">
+        <v>26</v>
+      </c>
+      <c r="E164" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>163</v>
+      </c>
+      <c r="B165">
+        <v>5</v>
+      </c>
+      <c r="C165">
+        <v>253</v>
+      </c>
+      <c r="D165">
+        <v>26</v>
+      </c>
+      <c r="E165" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <v>7</v>
+      </c>
+      <c r="C166">
+        <v>267</v>
+      </c>
+      <c r="D166">
+        <v>26</v>
+      </c>
+      <c r="E166" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>165</v>
+      </c>
+      <c r="B167">
+        <v>9</v>
+      </c>
+      <c r="C167">
+        <v>270</v>
+      </c>
+      <c r="D167">
+        <v>26</v>
+      </c>
+      <c r="E167" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>166</v>
+      </c>
+      <c r="B168">
+        <v>11</v>
+      </c>
+      <c r="C168">
+        <v>268</v>
+      </c>
+      <c r="D168">
+        <v>26</v>
+      </c>
+      <c r="E168" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>167</v>
+      </c>
+      <c r="B169">
+        <v>13</v>
+      </c>
+      <c r="C169">
+        <v>258</v>
+      </c>
+      <c r="D169">
+        <v>26</v>
+      </c>
+      <c r="E169" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>168</v>
+      </c>
+      <c r="B170">
+        <v>15</v>
+      </c>
+      <c r="C170">
+        <v>249</v>
+      </c>
+      <c r="D170">
+        <v>26</v>
+      </c>
+      <c r="E170" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <v>17</v>
+      </c>
+      <c r="C171">
+        <v>278</v>
+      </c>
+      <c r="D171">
+        <v>26</v>
+      </c>
+      <c r="E171" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <v>19</v>
+      </c>
+      <c r="C172">
+        <v>275</v>
+      </c>
+      <c r="D172">
+        <v>26</v>
+      </c>
+      <c r="E172" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>171</v>
+      </c>
+      <c r="B173">
+        <v>21</v>
+      </c>
+      <c r="C173">
+        <v>271</v>
+      </c>
+      <c r="D173">
+        <v>26</v>
+      </c>
+      <c r="E173" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>172</v>
+      </c>
+      <c r="B174">
+        <v>23</v>
+      </c>
+      <c r="C174">
+        <v>298</v>
+      </c>
+      <c r="D174">
+        <v>26</v>
+      </c>
+      <c r="E174" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>173</v>
+      </c>
+      <c r="B175">
+        <v>25</v>
+      </c>
+      <c r="C175">
+        <v>299</v>
+      </c>
+      <c r="D175">
+        <v>26</v>
+      </c>
+      <c r="E175" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>174</v>
+      </c>
+      <c r="B176">
+        <v>27</v>
+      </c>
+      <c r="C176">
+        <v>255</v>
+      </c>
+      <c r="D176">
+        <v>26</v>
+      </c>
+      <c r="E176" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>175</v>
+      </c>
+      <c r="B177">
+        <v>29</v>
+      </c>
+      <c r="C177">
+        <v>292</v>
+      </c>
+      <c r="D177">
+        <v>26</v>
+      </c>
+      <c r="E177" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>176</v>
+      </c>
+      <c r="B178">
+        <v>31</v>
+      </c>
+      <c r="C178">
+        <v>282</v>
+      </c>
+      <c r="D178">
+        <v>26</v>
+      </c>
+      <c r="E178" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>177</v>
+      </c>
+      <c r="B179">
+        <v>33</v>
+      </c>
+      <c r="C179">
+        <v>271</v>
+      </c>
+      <c r="D179">
+        <v>26</v>
+      </c>
+      <c r="E179" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>178</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <v>340</v>
+      </c>
+      <c r="D180">
+        <v>28</v>
+      </c>
+      <c r="E180" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>179</v>
+      </c>
+      <c r="B181">
+        <v>1</v>
+      </c>
+      <c r="C181">
+        <v>340</v>
+      </c>
+      <c r="D181">
+        <v>28</v>
+      </c>
+      <c r="E181" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>180</v>
+      </c>
+      <c r="B182">
+        <v>3</v>
+      </c>
+      <c r="C182">
+        <v>328</v>
+      </c>
+      <c r="D182">
+        <v>28</v>
+      </c>
+      <c r="E182" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>181</v>
+      </c>
+      <c r="B183">
+        <v>5</v>
+      </c>
+      <c r="C183">
+        <v>330</v>
+      </c>
+      <c r="D183">
+        <v>28</v>
+      </c>
+      <c r="E183" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <v>7</v>
+      </c>
+      <c r="C184">
+        <v>335</v>
+      </c>
+      <c r="D184">
+        <v>28</v>
+      </c>
+      <c r="E184" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>183</v>
+      </c>
+      <c r="B185">
+        <v>9</v>
+      </c>
+      <c r="C185">
+        <v>340</v>
+      </c>
+      <c r="D185">
+        <v>28</v>
+      </c>
+      <c r="E185" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>184</v>
+      </c>
+      <c r="B186">
+        <v>11</v>
+      </c>
+      <c r="C186">
+        <v>342</v>
+      </c>
+      <c r="D186">
+        <v>28</v>
+      </c>
+      <c r="E186" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>185</v>
+      </c>
+      <c r="B187">
+        <v>13</v>
+      </c>
+      <c r="C187">
+        <v>341</v>
+      </c>
+      <c r="D187">
+        <v>28</v>
+      </c>
+      <c r="E187" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>186</v>
+      </c>
+      <c r="B188">
+        <v>15</v>
+      </c>
+      <c r="C188">
+        <v>345</v>
+      </c>
+      <c r="D188">
+        <v>28</v>
+      </c>
+      <c r="E188" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>187</v>
+      </c>
+      <c r="B189">
+        <v>17</v>
+      </c>
+      <c r="C189">
+        <v>346</v>
+      </c>
+      <c r="D189">
+        <v>28</v>
+      </c>
+      <c r="E189" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>188</v>
+      </c>
+      <c r="B190">
+        <v>19</v>
+      </c>
+      <c r="C190">
+        <v>348</v>
+      </c>
+      <c r="D190">
+        <v>28</v>
+      </c>
+      <c r="E190" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>189</v>
+      </c>
+      <c r="B191">
+        <v>21</v>
+      </c>
+      <c r="C191">
+        <v>351</v>
+      </c>
+      <c r="D191">
+        <v>28</v>
+      </c>
+      <c r="E191" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>190</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>310</v>
+      </c>
+      <c r="D192">
+        <v>30</v>
+      </c>
+      <c r="E192" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>191</v>
+      </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="C193">
+        <v>305</v>
+      </c>
+      <c r="D193">
+        <v>30</v>
+      </c>
+      <c r="E193" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>192</v>
+      </c>
+      <c r="B194">
+        <v>3</v>
+      </c>
+      <c r="C194">
+        <v>309</v>
+      </c>
+      <c r="D194">
+        <v>30</v>
+      </c>
+      <c r="E194" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>193</v>
+      </c>
+      <c r="B195">
+        <v>5</v>
+      </c>
+      <c r="C195">
+        <v>326</v>
+      </c>
+      <c r="D195">
+        <v>30</v>
+      </c>
+      <c r="E195" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>194</v>
+      </c>
+      <c r="B196">
+        <v>7</v>
+      </c>
+      <c r="C196">
+        <v>335</v>
+      </c>
+      <c r="D196">
+        <v>30</v>
+      </c>
+      <c r="E196" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>195</v>
+      </c>
+      <c r="B197">
+        <v>9</v>
+      </c>
+      <c r="C197">
+        <v>355</v>
+      </c>
+      <c r="D197">
+        <v>30</v>
+      </c>
+      <c r="E197" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>196</v>
+      </c>
+      <c r="B198">
+        <v>11</v>
+      </c>
+      <c r="C198">
+        <v>375</v>
+      </c>
+      <c r="D198">
+        <v>30</v>
+      </c>
+      <c r="E198" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>197</v>
+      </c>
+      <c r="B199">
+        <v>13</v>
+      </c>
+      <c r="C199">
+        <v>384</v>
+      </c>
+      <c r="D199">
+        <v>30</v>
+      </c>
+      <c r="E199" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>198</v>
+      </c>
+      <c r="B200">
+        <v>15</v>
+      </c>
+      <c r="C200">
+        <v>393</v>
+      </c>
+      <c r="D200">
+        <v>30</v>
+      </c>
+      <c r="E200" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>199</v>
+      </c>
+      <c r="B201">
+        <v>17</v>
+      </c>
+      <c r="C201">
+        <v>408</v>
+      </c>
+      <c r="D201">
+        <v>30</v>
+      </c>
+      <c r="E201" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>200</v>
+      </c>
+      <c r="B202">
+        <v>19</v>
+      </c>
+      <c r="C202">
+        <v>413</v>
+      </c>
+      <c r="D202">
+        <v>30</v>
+      </c>
+      <c r="E202" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>201</v>
+      </c>
+      <c r="B203">
+        <v>21</v>
+      </c>
+      <c r="C203">
+        <v>416</v>
+      </c>
+      <c r="D203">
+        <v>30</v>
+      </c>
+      <c r="E203" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>202</v>
+      </c>
+      <c r="B204">
+        <v>23</v>
+      </c>
+      <c r="C204">
+        <v>418</v>
+      </c>
+      <c r="D204">
+        <v>30</v>
+      </c>
+      <c r="E204" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>203</v>
+      </c>
+      <c r="B205">
+        <v>0</v>
+      </c>
+      <c r="C205">
+        <v>327</v>
+      </c>
+      <c r="D205">
+        <v>32</v>
+      </c>
+      <c r="E205" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>204</v>
+      </c>
+      <c r="B206">
+        <v>1</v>
+      </c>
+      <c r="C206">
+        <v>380</v>
+      </c>
+      <c r="D206">
+        <v>32</v>
+      </c>
+      <c r="E206" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>205</v>
+      </c>
+      <c r="B207">
+        <v>3</v>
+      </c>
+      <c r="C207">
+        <v>390</v>
+      </c>
+      <c r="D207">
+        <v>32</v>
+      </c>
+      <c r="E207" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>206</v>
+      </c>
+      <c r="B208">
+        <v>5</v>
+      </c>
+      <c r="C208">
+        <v>415</v>
+      </c>
+      <c r="D208">
+        <v>32</v>
+      </c>
+      <c r="E208" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>207</v>
+      </c>
+      <c r="B209">
+        <v>7</v>
+      </c>
+      <c r="C209">
+        <v>420</v>
+      </c>
+      <c r="D209">
+        <v>32</v>
+      </c>
+      <c r="E209" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>208</v>
+      </c>
+      <c r="B210">
+        <v>9</v>
+      </c>
+      <c r="C210">
+        <v>432</v>
+      </c>
+      <c r="D210">
+        <v>32</v>
+      </c>
+      <c r="E210" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>209</v>
+      </c>
+      <c r="B211">
+        <v>11</v>
+      </c>
+      <c r="C211">
+        <v>443</v>
+      </c>
+      <c r="D211">
+        <v>32</v>
+      </c>
+      <c r="E211" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>210</v>
+      </c>
+      <c r="B212">
+        <v>13</v>
+      </c>
+      <c r="C212">
+        <v>455</v>
+      </c>
+      <c r="D212">
+        <v>32</v>
+      </c>
+      <c r="E212" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>211</v>
+      </c>
+      <c r="B213">
+        <v>15</v>
+      </c>
+      <c r="C213">
+        <v>465</v>
+      </c>
+      <c r="D213">
+        <v>32</v>
+      </c>
+      <c r="E213" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>212</v>
+      </c>
+      <c r="B214">
+        <v>17</v>
+      </c>
+      <c r="C214">
+        <v>473</v>
+      </c>
+      <c r="D214">
+        <v>32</v>
+      </c>
+      <c r="E214" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>213</v>
+      </c>
+      <c r="B215">
+        <v>19</v>
+      </c>
+      <c r="C215">
+        <v>488</v>
+      </c>
+      <c r="D215">
+        <v>32</v>
+      </c>
+      <c r="E215" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>214</v>
+      </c>
+      <c r="B216">
+        <v>21</v>
+      </c>
+      <c r="C216">
+        <v>486</v>
+      </c>
+      <c r="D216">
+        <v>32</v>
+      </c>
+      <c r="E216" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>215</v>
+      </c>
+      <c r="B217">
+        <v>23</v>
+      </c>
+      <c r="C217">
+        <v>495</v>
+      </c>
+      <c r="D217">
+        <v>32</v>
+      </c>
+      <c r="E217" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>216</v>
+      </c>
+      <c r="B218">
+        <v>25</v>
+      </c>
+      <c r="C218">
+        <v>514</v>
+      </c>
+      <c r="D218">
+        <v>32</v>
+      </c>
+      <c r="E218" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>217</v>
+      </c>
+      <c r="B219">
+        <v>0</v>
+      </c>
+      <c r="C219">
+        <v>301</v>
+      </c>
+      <c r="D219">
+        <v>34</v>
+      </c>
+      <c r="E219" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>218</v>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+      <c r="C220">
+        <v>360</v>
+      </c>
+      <c r="D220">
+        <v>34</v>
+      </c>
+      <c r="E220" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>219</v>
+      </c>
+      <c r="B221">
+        <v>3</v>
+      </c>
+      <c r="C221">
+        <v>380</v>
+      </c>
+      <c r="D221">
+        <v>34</v>
+      </c>
+      <c r="E221" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>220</v>
+      </c>
+      <c r="B222">
+        <v>5</v>
+      </c>
+      <c r="C222">
+        <v>388</v>
+      </c>
+      <c r="D222">
+        <v>34</v>
+      </c>
+      <c r="E222" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>221</v>
+      </c>
+      <c r="B223">
+        <v>7</v>
+      </c>
+      <c r="C223">
+        <v>395</v>
+      </c>
+      <c r="D223">
+        <v>34</v>
+      </c>
+      <c r="E223" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>222</v>
+      </c>
+      <c r="B224">
+        <v>9</v>
+      </c>
+      <c r="C224">
+        <v>415</v>
+      </c>
+      <c r="D224">
+        <v>34</v>
+      </c>
+      <c r="E224" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>223</v>
+      </c>
+      <c r="B225">
+        <v>11</v>
+      </c>
+      <c r="C225">
+        <v>417</v>
+      </c>
+      <c r="D225">
+        <v>34</v>
+      </c>
+      <c r="E225" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>224</v>
+      </c>
+      <c r="B226">
+        <v>13</v>
+      </c>
+      <c r="C226">
+        <v>426</v>
+      </c>
+      <c r="D226">
+        <v>34</v>
+      </c>
+      <c r="E226" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>225</v>
+      </c>
+      <c r="B227">
+        <v>15</v>
+      </c>
+      <c r="C227">
+        <v>428</v>
+      </c>
+      <c r="D227">
+        <v>34</v>
+      </c>
+      <c r="E227" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>226</v>
+      </c>
+      <c r="B228">
+        <v>17</v>
+      </c>
+      <c r="C228">
+        <v>444</v>
+      </c>
+      <c r="D228">
+        <v>34</v>
+      </c>
+      <c r="E228" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>227</v>
+      </c>
+      <c r="B229">
+        <v>19</v>
+      </c>
+      <c r="C229">
+        <v>446</v>
+      </c>
+      <c r="D229">
+        <v>34</v>
+      </c>
+      <c r="E229" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>228</v>
+      </c>
+      <c r="B230">
+        <v>21</v>
+      </c>
+      <c r="C230">
+        <v>448</v>
+      </c>
+      <c r="D230">
+        <v>34</v>
+      </c>
+      <c r="E230" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>229</v>
+      </c>
+      <c r="B231">
+        <v>23</v>
+      </c>
+      <c r="C231">
+        <v>457</v>
+      </c>
+      <c r="D231">
+        <v>34</v>
+      </c>
+      <c r="E231" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>230</v>
+      </c>
+      <c r="B232">
+        <v>25</v>
+      </c>
+      <c r="C232">
+        <v>464</v>
+      </c>
+      <c r="D232">
+        <v>34</v>
+      </c>
+      <c r="E232" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A233" s="2">
+        <v>231</v>
+      </c>
+      <c r="B233">
+        <v>0</v>
+      </c>
+      <c r="C233">
+        <v>376</v>
+      </c>
+      <c r="D233">
+        <v>36</v>
+      </c>
+      <c r="E233" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>232</v>
+      </c>
+      <c r="B234">
+        <v>1</v>
+      </c>
+      <c r="C234">
+        <v>376</v>
+      </c>
+      <c r="D234">
+        <v>36</v>
+      </c>
+      <c r="E234" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>233</v>
+      </c>
+      <c r="B235">
+        <v>3</v>
+      </c>
+      <c r="C235">
+        <v>354</v>
+      </c>
+      <c r="D235">
+        <v>36</v>
+      </c>
+      <c r="E235" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>234</v>
+      </c>
+      <c r="B236">
+        <v>5</v>
+      </c>
+      <c r="C236">
+        <v>364</v>
+      </c>
+      <c r="D236">
+        <v>36</v>
+      </c>
+      <c r="E236" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>235</v>
+      </c>
+      <c r="B237">
+        <v>7</v>
+      </c>
+      <c r="C237">
+        <v>365</v>
+      </c>
+      <c r="D237">
+        <v>36</v>
+      </c>
+      <c r="E237" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>236</v>
+      </c>
+      <c r="B238">
+        <v>9</v>
+      </c>
+      <c r="C238">
+        <v>388</v>
+      </c>
+      <c r="D238">
+        <v>36</v>
+      </c>
+      <c r="E238" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>237</v>
+      </c>
+      <c r="B239">
+        <v>11</v>
+      </c>
+      <c r="C239">
+        <v>384</v>
+      </c>
+      <c r="D239">
+        <v>36</v>
+      </c>
+      <c r="E239" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>238</v>
+      </c>
+      <c r="B240">
+        <v>13</v>
+      </c>
+      <c r="C240">
+        <v>410</v>
+      </c>
+      <c r="D240">
+        <v>36</v>
+      </c>
+      <c r="E240" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>239</v>
+      </c>
+      <c r="B241">
+        <v>15</v>
+      </c>
+      <c r="C241">
+        <v>413</v>
+      </c>
+      <c r="D241">
+        <v>36</v>
+      </c>
+      <c r="E241" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>240</v>
+      </c>
+      <c r="B242">
+        <v>17</v>
+      </c>
+      <c r="C242">
+        <v>424</v>
+      </c>
+      <c r="D242">
+        <v>36</v>
+      </c>
+      <c r="E242" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>241</v>
+      </c>
+      <c r="B243">
+        <v>19</v>
+      </c>
+      <c r="C243">
+        <v>433</v>
+      </c>
+      <c r="D243">
+        <v>36</v>
+      </c>
+      <c r="E243" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>242</v>
+      </c>
+      <c r="B244">
+        <v>21</v>
+      </c>
+      <c r="C244">
+        <v>447</v>
+      </c>
+      <c r="D244">
+        <v>36</v>
+      </c>
+      <c r="E244" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>243</v>
+      </c>
+      <c r="B245">
+        <v>0</v>
+      </c>
+      <c r="C245">
+        <v>406</v>
+      </c>
+      <c r="D245">
+        <v>38</v>
+      </c>
+      <c r="E245" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>244</v>
+      </c>
+      <c r="B246">
+        <v>1</v>
+      </c>
+      <c r="C246">
+        <v>406</v>
+      </c>
+      <c r="D246">
+        <v>38</v>
+      </c>
+      <c r="E246" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>245</v>
+      </c>
+      <c r="B247">
+        <v>3</v>
+      </c>
+      <c r="C247">
+        <v>387</v>
+      </c>
+      <c r="D247">
+        <v>38</v>
+      </c>
+      <c r="E247" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>246</v>
+      </c>
+      <c r="B248">
+        <v>5</v>
+      </c>
+      <c r="C248">
+        <v>403</v>
+      </c>
+      <c r="D248">
+        <v>38</v>
+      </c>
+      <c r="E248" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>247</v>
+      </c>
+      <c r="B249">
+        <v>7</v>
+      </c>
+      <c r="C249">
+        <v>386</v>
+      </c>
+      <c r="D249">
+        <v>38</v>
+      </c>
+      <c r="E249" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>248</v>
+      </c>
+      <c r="B250">
+        <v>9</v>
+      </c>
+      <c r="C250">
+        <v>416</v>
+      </c>
+      <c r="D250">
+        <v>38</v>
+      </c>
+      <c r="E250" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>249</v>
+      </c>
+      <c r="B251">
+        <v>11</v>
+      </c>
+      <c r="C251">
+        <v>424</v>
+      </c>
+      <c r="D251">
+        <v>38</v>
+      </c>
+      <c r="E251" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>250</v>
+      </c>
+      <c r="B252">
+        <v>13</v>
+      </c>
+      <c r="C252">
+        <v>450</v>
+      </c>
+      <c r="D252">
+        <v>38</v>
+      </c>
+      <c r="E252" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>251</v>
+      </c>
+      <c r="B253">
+        <v>15</v>
+      </c>
+      <c r="C253">
+        <v>450</v>
+      </c>
+      <c r="D253">
+        <v>38</v>
+      </c>
+      <c r="E253" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>252</v>
+      </c>
+      <c r="B254">
+        <v>17</v>
+      </c>
+      <c r="C254">
+        <v>460</v>
+      </c>
+      <c r="D254">
+        <v>38</v>
+      </c>
+      <c r="E254" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>253</v>
+      </c>
+      <c r="B255">
+        <v>19</v>
+      </c>
+      <c r="C255">
+        <v>464</v>
+      </c>
+      <c r="D255">
+        <v>38</v>
+      </c>
+      <c r="E255" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A256" s="2">
+        <v>254</v>
+      </c>
+      <c r="B256">
+        <v>21</v>
+      </c>
+      <c r="C256">
+        <v>478</v>
+      </c>
+      <c r="D256">
+        <v>38</v>
+      </c>
+      <c r="E256" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A257" s="2">
+        <v>255</v>
+      </c>
+      <c r="B257">
+        <v>0</v>
+      </c>
+      <c r="C257">
+        <v>370</v>
+      </c>
+      <c r="D257">
+        <v>40</v>
+      </c>
+      <c r="E257" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A258" s="2">
+        <v>256</v>
+      </c>
+      <c r="B258">
+        <v>1</v>
+      </c>
+      <c r="C258">
+        <v>375</v>
+      </c>
+      <c r="D258">
+        <v>40</v>
+      </c>
+      <c r="E258" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A259" s="2">
+        <v>257</v>
+      </c>
+      <c r="B259">
+        <v>3</v>
+      </c>
+      <c r="C259">
+        <v>385</v>
+      </c>
+      <c r="D259">
+        <v>40</v>
+      </c>
+      <c r="E259" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>258</v>
+      </c>
+      <c r="B260">
+        <v>5</v>
+      </c>
+      <c r="C260">
+        <v>392</v>
+      </c>
+      <c r="D260">
+        <v>40</v>
+      </c>
+      <c r="E260" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>259</v>
+      </c>
+      <c r="B261">
+        <v>7</v>
+      </c>
+      <c r="C261">
+        <v>402</v>
+      </c>
+      <c r="D261">
+        <v>40</v>
+      </c>
+      <c r="E261" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>260</v>
+      </c>
+      <c r="B262">
+        <v>9</v>
+      </c>
+      <c r="C262">
+        <v>405</v>
+      </c>
+      <c r="D262">
+        <v>40</v>
+      </c>
+      <c r="E262" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A263" s="2">
+        <v>261</v>
+      </c>
+      <c r="B263">
+        <v>11</v>
+      </c>
+      <c r="C263">
+        <v>407</v>
+      </c>
+      <c r="D263">
+        <v>40</v>
+      </c>
+      <c r="E263" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A264" s="2">
+        <v>262</v>
+      </c>
+      <c r="B264">
+        <v>13</v>
+      </c>
+      <c r="C264">
+        <v>415</v>
+      </c>
+      <c r="D264">
+        <v>40</v>
+      </c>
+      <c r="E264" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A265" s="2">
+        <v>263</v>
+      </c>
+      <c r="B265">
+        <v>15</v>
+      </c>
+      <c r="C265">
+        <v>417</v>
+      </c>
+      <c r="D265">
+        <v>40</v>
+      </c>
+      <c r="E265" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A266" s="2">
+        <v>264</v>
+      </c>
+      <c r="B266">
+        <v>17</v>
+      </c>
+      <c r="C266">
+        <v>429</v>
+      </c>
+      <c r="D266">
+        <v>40</v>
+      </c>
+      <c r="E266" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A267" s="2">
+        <v>265</v>
+      </c>
+      <c r="B267">
+        <v>19</v>
+      </c>
+      <c r="C267">
+        <v>437</v>
+      </c>
+      <c r="D267">
+        <v>40</v>
+      </c>
+      <c r="E267" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A268" s="2">
+        <v>266</v>
+      </c>
+      <c r="B268">
+        <v>21</v>
+      </c>
+      <c r="C268">
+        <v>450</v>
+      </c>
+      <c r="D268">
+        <v>40</v>
+      </c>
+      <c r="E268" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A269" s="2">
+        <v>267</v>
+      </c>
+      <c r="B269">
+        <v>23</v>
+      </c>
+      <c r="C269">
+        <v>450</v>
+      </c>
+      <c r="D269">
+        <v>40</v>
+      </c>
+      <c r="E269" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A270" s="2">
+        <v>268</v>
+      </c>
+      <c r="B270">
+        <v>25</v>
+      </c>
+      <c r="C270">
+        <v>452</v>
+      </c>
+      <c r="D270">
+        <v>40</v>
+      </c>
+      <c r="E270" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>269</v>
+      </c>
+      <c r="B271">
+        <v>27</v>
+      </c>
+      <c r="C271">
+        <v>465</v>
+      </c>
+      <c r="D271">
+        <v>40</v>
+      </c>
+      <c r="E271" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>270</v>
+      </c>
+      <c r="B272">
+        <v>0</v>
+      </c>
+      <c r="C272">
+        <v>424</v>
+      </c>
+      <c r="D272">
+        <v>42</v>
+      </c>
+      <c r="E272" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A273" s="2">
+        <v>271</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+      <c r="C273">
+        <v>424</v>
+      </c>
+      <c r="D273">
+        <v>42</v>
+      </c>
+      <c r="E273" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A274" s="2">
+        <v>272</v>
+      </c>
+      <c r="B274">
+        <v>3</v>
+      </c>
+      <c r="C274">
+        <v>405</v>
+      </c>
+      <c r="D274">
+        <v>42</v>
+      </c>
+      <c r="E274" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A275" s="2">
+        <v>273</v>
+      </c>
+      <c r="B275">
+        <v>5</v>
+      </c>
+      <c r="C275">
+        <v>413</v>
+      </c>
+      <c r="D275">
+        <v>42</v>
+      </c>
+      <c r="E275" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A276" s="2">
+        <v>274</v>
+      </c>
+      <c r="B276">
+        <v>7</v>
+      </c>
+      <c r="C276">
+        <v>429</v>
+      </c>
+      <c r="D276">
+        <v>42</v>
+      </c>
+      <c r="E276" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A277" s="2">
+        <v>275</v>
+      </c>
+      <c r="B277">
+        <v>9</v>
+      </c>
+      <c r="C277">
+        <v>436</v>
+      </c>
+      <c r="D277">
+        <v>42</v>
+      </c>
+      <c r="E277" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A278" s="2">
+        <v>276</v>
+      </c>
+      <c r="B278">
+        <v>11</v>
+      </c>
+      <c r="C278">
+        <v>432</v>
+      </c>
+      <c r="D278">
+        <v>42</v>
+      </c>
+      <c r="E278" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>277</v>
+      </c>
+      <c r="B279">
+        <v>13</v>
+      </c>
+      <c r="C279">
+        <v>455</v>
+      </c>
+      <c r="D279">
+        <v>42</v>
+      </c>
+      <c r="E279" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
+        <v>278</v>
+      </c>
+      <c r="B280">
+        <v>15</v>
+      </c>
+      <c r="C280">
+        <v>470</v>
+      </c>
+      <c r="D280">
+        <v>42</v>
+      </c>
+      <c r="E280" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A281" s="2">
+        <v>279</v>
+      </c>
+      <c r="B281">
+        <v>17</v>
+      </c>
+      <c r="C281">
+        <v>479</v>
+      </c>
+      <c r="D281">
+        <v>42</v>
+      </c>
+      <c r="E281" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A282" s="2">
+        <v>280</v>
+      </c>
+      <c r="B282">
+        <v>19</v>
+      </c>
+      <c r="C282">
+        <v>486</v>
+      </c>
+      <c r="D282">
+        <v>42</v>
+      </c>
+      <c r="E282" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A283" s="2">
+        <v>281</v>
+      </c>
+      <c r="B283">
+        <v>21</v>
+      </c>
+      <c r="C283">
+        <v>496</v>
+      </c>
+      <c r="D283">
+        <v>42</v>
+      </c>
+      <c r="E283" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A284" s="2">
+        <v>282</v>
+      </c>
+      <c r="B284">
+        <v>23</v>
+      </c>
+      <c r="C284">
+        <v>505</v>
+      </c>
+      <c r="D284">
+        <v>42</v>
+      </c>
+      <c r="E284" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A285" s="2">
+        <v>283</v>
+      </c>
+      <c r="B285">
+        <v>25</v>
+      </c>
+      <c r="C285">
+        <v>507</v>
+      </c>
+      <c r="D285">
+        <v>42</v>
+      </c>
+      <c r="E285" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A286" s="2">
+        <v>284</v>
+      </c>
+      <c r="B286">
+        <v>27</v>
+      </c>
+      <c r="C286">
+        <v>513</v>
+      </c>
+      <c r="D286">
+        <v>42</v>
+      </c>
+      <c r="E286" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A287" s="2">
+        <v>285</v>
+      </c>
+      <c r="B287">
+        <v>29</v>
+      </c>
+      <c r="C287">
+        <v>518</v>
+      </c>
+      <c r="D287">
+        <v>42</v>
+      </c>
+      <c r="E287" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bug-fix : plot.pro_bar_data ask min_sample_N > 0\ make sure None meaning combi will not exist
</commit_message>
<xml_diff>
--- a/data/plot.xlsx
+++ b/data/plot.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_Progs\BA\Python\BA_PY\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C038BA0-57D8-4624-80B0-1C5CCB49B5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A327FEC-ED9B-4791-A3E0-DEE0D7C6B38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="1944" windowWidth="17280" windowHeight="10320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="xm" sheetId="1" r:id="rId1"/>
     <sheet name="ym" sheetId="2" r:id="rId2"/>
     <sheet name="peak" sheetId="3" r:id="rId3"/>
     <sheet name="weight" sheetId="4" r:id="rId4"/>
+    <sheet name="MWM" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="125">
   <si>
     <t>solution</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,6 +182,261 @@
   <si>
     <t>Exp</t>
   </si>
+  <si>
+    <t>Animal No.</t>
+  </si>
+  <si>
+    <t>Trial Type</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Start time</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>OutRing time</t>
+  </si>
+  <si>
+    <t>OutRing len</t>
+  </si>
+  <si>
+    <t>MidRing time</t>
+  </si>
+  <si>
+    <t>MidRing len</t>
+  </si>
+  <si>
+    <t>InnerRing time</t>
+  </si>
+  <si>
+    <t>InnerRing len</t>
+  </si>
+  <si>
+    <t>Quadrant-I time</t>
+  </si>
+  <si>
+    <t>Quadrant-I len</t>
+  </si>
+  <si>
+    <t>Quadrant-II time</t>
+  </si>
+  <si>
+    <t>Quadrant-II len</t>
+  </si>
+  <si>
+    <t>Quadrant-III time</t>
+  </si>
+  <si>
+    <t>Quadrant-III len</t>
+  </si>
+  <si>
+    <t>Quadrant-IV  time</t>
+  </si>
+  <si>
+    <t>Quadrant-IV  len</t>
+  </si>
+  <si>
+    <t>Plat-stayed time</t>
+  </si>
+  <si>
+    <t>Plat-stayed len</t>
+  </si>
+  <si>
+    <t>Effective region time</t>
+  </si>
+  <si>
+    <t>Effective region len</t>
+  </si>
+  <si>
+    <t>Total len</t>
+  </si>
+  <si>
+    <t>Avg speed</t>
+  </si>
+  <si>
+    <t>Orientation angle</t>
+  </si>
+  <si>
+    <t>Across plat times</t>
+  </si>
+  <si>
+    <t>Across effective region times</t>
+  </si>
+  <si>
+    <t>Phase-1 effective rate</t>
+  </si>
+  <si>
+    <t>Phase-2 effective rate</t>
+  </si>
+  <si>
+    <t>Phase-3 effective rate</t>
+  </si>
+  <si>
+    <t>Phase-4 effective rate</t>
+  </si>
+  <si>
+    <t>Phase-5 effective rate</t>
+  </si>
+  <si>
+    <t>Phase-6 effective rate</t>
+  </si>
+  <si>
+    <t>First entry time</t>
+  </si>
+  <si>
+    <t>First Entry Len</t>
+  </si>
+  <si>
+    <t>First Entry Speed</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>Animal Type</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Place Navigation</t>
+  </si>
+  <si>
+    <t>day0</t>
+  </si>
+  <si>
+    <t>2023-4-1-18-55-21</t>
+  </si>
+  <si>
+    <t>No memo</t>
+  </si>
+  <si>
+    <t>2023-4-1-19-0-11</t>
+  </si>
+  <si>
+    <t>2023-4-1-19-5-20</t>
+  </si>
+  <si>
+    <t>2023-4-1-19-10-10</t>
+  </si>
+  <si>
+    <t>2023-4-1-19-15-39</t>
+  </si>
+  <si>
+    <t>2023-4-1-19-21-30</t>
+  </si>
+  <si>
+    <t>2023-4-1-19-25-12</t>
+  </si>
+  <si>
+    <t>No Memo</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>day1</t>
+  </si>
+  <si>
+    <t>2023-4-2-21-3-28</t>
+  </si>
+  <si>
+    <t>2023-4-2-21-11-16</t>
+  </si>
+  <si>
+    <t>2023-4-2-21-14-12</t>
+  </si>
+  <si>
+    <t>2023-4-2-21-18-6</t>
+  </si>
+  <si>
+    <t>2023-4-2-21-21-1</t>
+  </si>
+  <si>
+    <t>2023-4-2-21-23-52</t>
+  </si>
+  <si>
+    <t>2023-4-2-21-26-41</t>
+  </si>
+  <si>
+    <t>day2</t>
+  </si>
+  <si>
+    <t>2023-4-3-15-35-10</t>
+  </si>
+  <si>
+    <t>2023-4-3-15-38-48</t>
+  </si>
+  <si>
+    <t>2023-4-3-15-41-17</t>
+  </si>
+  <si>
+    <t>2023-4-3-15-43-20</t>
+  </si>
+  <si>
+    <t>2023-4-3-15-47-14</t>
+  </si>
+  <si>
+    <t>2023-4-3-15-50-12</t>
+  </si>
+  <si>
+    <t>2023-4-3-15-54-4</t>
+  </si>
+  <si>
+    <t>day3</t>
+  </si>
+  <si>
+    <t>2023-4-4-15-20-35</t>
+  </si>
+  <si>
+    <t>2023-4-4-15-24-20</t>
+  </si>
+  <si>
+    <t>2023-4-4-15-26-55</t>
+  </si>
+  <si>
+    <t>2023-4-4-15-29-55</t>
+  </si>
+  <si>
+    <t>2023-4-4-15-32-43</t>
+  </si>
+  <si>
+    <t>2023-4-4-15-36-1</t>
+  </si>
+  <si>
+    <t>2023-4-4-15-38-31</t>
+  </si>
+  <si>
+    <t>Space Exploration</t>
+  </si>
+  <si>
+    <t>day4</t>
+  </si>
+  <si>
+    <t>2023-4-5-21-16-14</t>
+  </si>
+  <si>
+    <t>2023-4-5-21-20-29</t>
+  </si>
+  <si>
+    <t>2023-4-5-21-25-9</t>
+  </si>
+  <si>
+    <t>2023-4-5-21-29-25</t>
+  </si>
+  <si>
+    <t>2023-4-5-21-32-29</t>
+  </si>
+  <si>
+    <t>2023-4-5-21-35-36</t>
+  </si>
+  <si>
+    <t>2023-4-5-21-38-23</t>
+  </si>
 </sst>
 </file>
 
@@ -244,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,6 +508,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -7819,7 +8076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579F8FC8-BF69-49E4-886E-5CD872A47A8A}">
   <dimension ref="A1:E287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -12705,4 +12962,4518 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1894524E-87AF-418E-BEF3-AA46814B8B6A}">
+  <dimension ref="A1:AO36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2">
+        <v>120.777</v>
+      </c>
+      <c r="G2">
+        <v>102.52200000000001</v>
+      </c>
+      <c r="H2">
+        <v>1414.0029999999999</v>
+      </c>
+      <c r="I2">
+        <v>14.532</v>
+      </c>
+      <c r="J2">
+        <v>309.28699999999998</v>
+      </c>
+      <c r="K2">
+        <v>3.7229999999999999</v>
+      </c>
+      <c r="L2">
+        <v>75.941000000000003</v>
+      </c>
+      <c r="M2">
+        <v>27.251999999999999</v>
+      </c>
+      <c r="N2">
+        <v>412.25400000000002</v>
+      </c>
+      <c r="O2">
+        <v>38.676000000000002</v>
+      </c>
+      <c r="P2">
+        <v>556.47699999999998</v>
+      </c>
+      <c r="Q2">
+        <v>32.356999999999999</v>
+      </c>
+      <c r="R2">
+        <v>475.62400000000002</v>
+      </c>
+      <c r="S2">
+        <v>22.492000000000001</v>
+      </c>
+      <c r="T2">
+        <v>354.87700000000001</v>
+      </c>
+      <c r="U2">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="V2">
+        <v>2.6080000000000001</v>
+      </c>
+      <c r="W2">
+        <v>3.0590000000000002</v>
+      </c>
+      <c r="X2">
+        <v>45.405999999999999</v>
+      </c>
+      <c r="Y2">
+        <v>1799.232</v>
+      </c>
+      <c r="Z2">
+        <v>14.897</v>
+      </c>
+      <c r="AA2">
+        <v>22.957999999999998</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="AK2">
+        <v>298.93900000000002</v>
+      </c>
+      <c r="AL2">
+        <v>17.18</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN2" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3">
+        <v>121.54600000000001</v>
+      </c>
+      <c r="G3">
+        <v>104.712</v>
+      </c>
+      <c r="H3">
+        <v>1849.5340000000001</v>
+      </c>
+      <c r="I3">
+        <v>13.226000000000001</v>
+      </c>
+      <c r="J3">
+        <v>285.63400000000001</v>
+      </c>
+      <c r="K3">
+        <v>3.6080000000000001</v>
+      </c>
+      <c r="L3">
+        <v>100.873</v>
+      </c>
+      <c r="M3">
+        <v>20.609000000000002</v>
+      </c>
+      <c r="N3">
+        <v>398.77499999999998</v>
+      </c>
+      <c r="O3">
+        <v>12.467000000000001</v>
+      </c>
+      <c r="P3">
+        <v>227.99199999999999</v>
+      </c>
+      <c r="Q3">
+        <v>51.764000000000003</v>
+      </c>
+      <c r="R3">
+        <v>879.30399999999997</v>
+      </c>
+      <c r="S3">
+        <v>36.706000000000003</v>
+      </c>
+      <c r="T3">
+        <v>729.97</v>
+      </c>
+      <c r="U3">
+        <v>1.8560000000000001</v>
+      </c>
+      <c r="V3">
+        <v>18.710999999999999</v>
+      </c>
+      <c r="W3">
+        <v>6.008</v>
+      </c>
+      <c r="X3">
+        <v>86.650999999999996</v>
+      </c>
+      <c r="Y3">
+        <v>2236.0410000000002</v>
+      </c>
+      <c r="Z3">
+        <v>18.396999999999998</v>
+      </c>
+      <c r="AA3">
+        <v>8.8109999999999999</v>
+      </c>
+      <c r="AB3">
+        <v>4</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AE3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AJ3">
+        <v>14.5</v>
+      </c>
+      <c r="AK3">
+        <v>306.55799999999999</v>
+      </c>
+      <c r="AL3">
+        <v>21.141999999999999</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4">
+        <v>63.679000000000002</v>
+      </c>
+      <c r="G4">
+        <v>31.29</v>
+      </c>
+      <c r="H4">
+        <v>536.01499999999999</v>
+      </c>
+      <c r="I4">
+        <v>26.03</v>
+      </c>
+      <c r="J4">
+        <v>464.43299999999999</v>
+      </c>
+      <c r="K4">
+        <v>6.359</v>
+      </c>
+      <c r="L4">
+        <v>126.696</v>
+      </c>
+      <c r="M4">
+        <v>19.161999999999999</v>
+      </c>
+      <c r="N4">
+        <v>307.75099999999998</v>
+      </c>
+      <c r="O4">
+        <v>9.8140000000000001</v>
+      </c>
+      <c r="P4">
+        <v>156.32300000000001</v>
+      </c>
+      <c r="Q4">
+        <v>19.204000000000001</v>
+      </c>
+      <c r="R4">
+        <v>357.43400000000003</v>
+      </c>
+      <c r="S4">
+        <v>15.499000000000001</v>
+      </c>
+      <c r="T4">
+        <v>305.637</v>
+      </c>
+      <c r="U4">
+        <v>2.8519999999999999</v>
+      </c>
+      <c r="V4">
+        <v>38.935000000000002</v>
+      </c>
+      <c r="W4">
+        <v>6.1349999999999998</v>
+      </c>
+      <c r="X4">
+        <v>87.587999999999994</v>
+      </c>
+      <c r="Y4">
+        <v>1127.144</v>
+      </c>
+      <c r="Z4">
+        <v>17.7</v>
+      </c>
+      <c r="AA4">
+        <v>137.858</v>
+      </c>
+      <c r="AB4">
+        <v>4</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0.216</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="AJ4">
+        <v>36.4</v>
+      </c>
+      <c r="AK4">
+        <v>703.61199999999997</v>
+      </c>
+      <c r="AL4">
+        <v>19.329999999999998</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN4" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5">
+        <v>121.31699999999999</v>
+      </c>
+      <c r="G5">
+        <v>88.992000000000004</v>
+      </c>
+      <c r="H5">
+        <v>1453.135</v>
+      </c>
+      <c r="I5">
+        <v>26.329000000000001</v>
+      </c>
+      <c r="J5">
+        <v>518.423</v>
+      </c>
+      <c r="K5">
+        <v>5.9960000000000004</v>
+      </c>
+      <c r="L5">
+        <v>131.76</v>
+      </c>
+      <c r="M5">
+        <v>18.445</v>
+      </c>
+      <c r="N5">
+        <v>293.10599999999999</v>
+      </c>
+      <c r="O5">
+        <v>24.686</v>
+      </c>
+      <c r="P5">
+        <v>413.37900000000002</v>
+      </c>
+      <c r="Q5">
+        <v>41.402999999999999</v>
+      </c>
+      <c r="R5">
+        <v>665.91899999999998</v>
+      </c>
+      <c r="S5">
+        <v>36.783000000000001</v>
+      </c>
+      <c r="T5">
+        <v>730.91399999999999</v>
+      </c>
+      <c r="U5">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="V5">
+        <v>13.71</v>
+      </c>
+      <c r="W5">
+        <v>6.8689999999999998</v>
+      </c>
+      <c r="X5">
+        <v>95.009</v>
+      </c>
+      <c r="Y5">
+        <v>2103.3180000000002</v>
+      </c>
+      <c r="Z5">
+        <v>17.337</v>
+      </c>
+      <c r="AA5">
+        <v>3.948</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AC5">
+        <v>4</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AF5">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AG5">
+        <v>0.129</v>
+      </c>
+      <c r="AH5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AI5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AJ5">
+        <v>36</v>
+      </c>
+      <c r="AK5">
+        <v>841.82399999999996</v>
+      </c>
+      <c r="AL5">
+        <v>23.384</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN5" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6">
+        <v>121.53700000000001</v>
+      </c>
+      <c r="G6">
+        <v>95.850999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1771.3409999999999</v>
+      </c>
+      <c r="I6">
+        <v>18.73</v>
+      </c>
+      <c r="J6">
+        <v>388.70600000000002</v>
+      </c>
+      <c r="K6">
+        <v>6.9560000000000004</v>
+      </c>
+      <c r="L6">
+        <v>154.054</v>
+      </c>
+      <c r="M6">
+        <v>28.504000000000001</v>
+      </c>
+      <c r="N6">
+        <v>534.97900000000004</v>
+      </c>
+      <c r="O6">
+        <v>25.664000000000001</v>
+      </c>
+      <c r="P6">
+        <v>536.64300000000003</v>
+      </c>
+      <c r="Q6">
+        <v>39.941000000000003</v>
+      </c>
+      <c r="R6">
+        <v>673.09799999999996</v>
+      </c>
+      <c r="S6">
+        <v>27.428000000000001</v>
+      </c>
+      <c r="T6">
+        <v>569.38099999999997</v>
+      </c>
+      <c r="U6">
+        <v>1.536</v>
+      </c>
+      <c r="V6">
+        <v>20.806999999999999</v>
+      </c>
+      <c r="W6">
+        <v>5.3550000000000004</v>
+      </c>
+      <c r="X6">
+        <v>88.757999999999996</v>
+      </c>
+      <c r="Y6">
+        <v>2314.1010000000001</v>
+      </c>
+      <c r="Z6">
+        <v>19.04</v>
+      </c>
+      <c r="AA6">
+        <v>82.756</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AC6">
+        <v>4</v>
+      </c>
+      <c r="AD6">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AE6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AF6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AG6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AH6">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>47.9</v>
+      </c>
+      <c r="AK6">
+        <v>1054.442</v>
+      </c>
+      <c r="AL6">
+        <v>22.013000000000002</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN6" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7">
+        <v>121.54</v>
+      </c>
+      <c r="G7">
+        <v>86.173000000000002</v>
+      </c>
+      <c r="H7">
+        <v>1716.1969999999999</v>
+      </c>
+      <c r="I7">
+        <v>27.638000000000002</v>
+      </c>
+      <c r="J7">
+        <v>613.08199999999999</v>
+      </c>
+      <c r="K7">
+        <v>7.7290000000000001</v>
+      </c>
+      <c r="L7">
+        <v>180.37100000000001</v>
+      </c>
+      <c r="M7">
+        <v>35.491999999999997</v>
+      </c>
+      <c r="N7">
+        <v>734.15700000000004</v>
+      </c>
+      <c r="O7">
+        <v>47.034999999999997</v>
+      </c>
+      <c r="P7">
+        <v>931.10299999999995</v>
+      </c>
+      <c r="Q7">
+        <v>28.859000000000002</v>
+      </c>
+      <c r="R7">
+        <v>611.25900000000001</v>
+      </c>
+      <c r="S7">
+        <v>10.154</v>
+      </c>
+      <c r="T7">
+        <v>233.13200000000001</v>
+      </c>
+      <c r="U7">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="V7">
+        <v>5.7</v>
+      </c>
+      <c r="W7">
+        <v>9.1579999999999995</v>
+      </c>
+      <c r="X7">
+        <v>186.792</v>
+      </c>
+      <c r="Y7">
+        <v>2509.6509999999998</v>
+      </c>
+      <c r="Z7">
+        <v>20.649000000000001</v>
+      </c>
+      <c r="AA7">
+        <v>62.070999999999998</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>10</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AF7">
+        <v>0.151</v>
+      </c>
+      <c r="AG7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AH7">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AI7">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AJ7">
+        <v>24.6</v>
+      </c>
+      <c r="AK7">
+        <v>556.55399999999997</v>
+      </c>
+      <c r="AL7">
+        <v>22.623999999999999</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN7" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8">
+        <v>121.541</v>
+      </c>
+      <c r="G8">
+        <v>92.953999999999994</v>
+      </c>
+      <c r="H8">
+        <v>1665.6659999999999</v>
+      </c>
+      <c r="I8">
+        <v>21.239000000000001</v>
+      </c>
+      <c r="J8">
+        <v>423.42700000000002</v>
+      </c>
+      <c r="K8">
+        <v>7.3479999999999999</v>
+      </c>
+      <c r="L8">
+        <v>164.04499999999999</v>
+      </c>
+      <c r="M8">
+        <v>31.984999999999999</v>
+      </c>
+      <c r="N8">
+        <v>582.00400000000002</v>
+      </c>
+      <c r="O8">
+        <v>34.411000000000001</v>
+      </c>
+      <c r="P8">
+        <v>628.58000000000004</v>
+      </c>
+      <c r="Q8">
+        <v>20.843</v>
+      </c>
+      <c r="R8">
+        <v>383.892</v>
+      </c>
+      <c r="S8">
+        <v>34.302</v>
+      </c>
+      <c r="T8">
+        <v>658.66</v>
+      </c>
+      <c r="U8">
+        <v>2.948</v>
+      </c>
+      <c r="V8">
+        <v>32.94</v>
+      </c>
+      <c r="W8">
+        <v>7.444</v>
+      </c>
+      <c r="X8">
+        <v>99.888000000000005</v>
+      </c>
+      <c r="Y8">
+        <v>2253.1370000000002</v>
+      </c>
+      <c r="Z8">
+        <v>18.538</v>
+      </c>
+      <c r="AA8">
+        <v>67.766999999999996</v>
+      </c>
+      <c r="AB8">
+        <v>3</v>
+      </c>
+      <c r="AC8">
+        <v>2</v>
+      </c>
+      <c r="AD8">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AE8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AF8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AI8">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AJ8">
+        <v>5.7</v>
+      </c>
+      <c r="AK8">
+        <v>112.684</v>
+      </c>
+      <c r="AL8">
+        <v>19.768999999999998</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9">
+        <v>121.55</v>
+      </c>
+      <c r="G9">
+        <v>109.447</v>
+      </c>
+      <c r="H9">
+        <v>2253.5790000000002</v>
+      </c>
+      <c r="I9">
+        <v>9.3010000000000002</v>
+      </c>
+      <c r="J9">
+        <v>265.51499999999999</v>
+      </c>
+      <c r="K9">
+        <v>2.802</v>
+      </c>
+      <c r="L9">
+        <v>72.290000000000006</v>
+      </c>
+      <c r="M9">
+        <v>32.642000000000003</v>
+      </c>
+      <c r="N9">
+        <v>667.57600000000002</v>
+      </c>
+      <c r="O9">
+        <v>30.181000000000001</v>
+      </c>
+      <c r="P9">
+        <v>644.30100000000004</v>
+      </c>
+      <c r="Q9">
+        <v>25.963000000000001</v>
+      </c>
+      <c r="R9">
+        <v>570.60299999999995</v>
+      </c>
+      <c r="S9">
+        <v>32.764000000000003</v>
+      </c>
+      <c r="T9">
+        <v>708.90599999999995</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="X9">
+        <v>17.584</v>
+      </c>
+      <c r="Y9">
+        <v>2591.3850000000002</v>
+      </c>
+      <c r="Z9">
+        <v>21.318999999999999</v>
+      </c>
+      <c r="AA9">
+        <v>135.785</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10">
+        <v>36.695</v>
+      </c>
+      <c r="G10">
+        <v>21.402999999999999</v>
+      </c>
+      <c r="H10">
+        <v>459.32299999999998</v>
+      </c>
+      <c r="I10">
+        <v>11.99</v>
+      </c>
+      <c r="J10">
+        <v>274.18299999999999</v>
+      </c>
+      <c r="K10">
+        <v>3.302</v>
+      </c>
+      <c r="L10">
+        <v>160.185</v>
+      </c>
+      <c r="M10">
+        <v>6.9630000000000001</v>
+      </c>
+      <c r="N10">
+        <v>247.173</v>
+      </c>
+      <c r="O10">
+        <v>5.69</v>
+      </c>
+      <c r="P10">
+        <v>111.806</v>
+      </c>
+      <c r="Q10">
+        <v>12.301</v>
+      </c>
+      <c r="R10">
+        <v>237.05500000000001</v>
+      </c>
+      <c r="S10">
+        <v>11.741</v>
+      </c>
+      <c r="T10">
+        <v>297.65600000000001</v>
+      </c>
+      <c r="U10">
+        <v>0.878</v>
+      </c>
+      <c r="V10">
+        <v>13.781000000000001</v>
+      </c>
+      <c r="W10">
+        <v>5.7830000000000004</v>
+      </c>
+      <c r="X10">
+        <v>82.227000000000004</v>
+      </c>
+      <c r="Y10">
+        <v>893.69</v>
+      </c>
+      <c r="Z10">
+        <v>24.355</v>
+      </c>
+      <c r="AA10">
+        <v>20.030999999999999</v>
+      </c>
+      <c r="AB10">
+        <v>7</v>
+      </c>
+      <c r="AC10">
+        <v>2</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AF10">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0.748</v>
+      </c>
+      <c r="AJ10">
+        <v>30.9</v>
+      </c>
+      <c r="AK10">
+        <v>855.93299999999999</v>
+      </c>
+      <c r="AL10">
+        <v>27.7</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11">
+        <v>22.385000000000002</v>
+      </c>
+      <c r="G11">
+        <v>7.8620000000000001</v>
+      </c>
+      <c r="H11">
+        <v>159.05600000000001</v>
+      </c>
+      <c r="I11">
+        <v>13.865</v>
+      </c>
+      <c r="J11">
+        <v>179.511</v>
+      </c>
+      <c r="K11">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="L11">
+        <v>21.579000000000001</v>
+      </c>
+      <c r="M11">
+        <v>4.4729999999999999</v>
+      </c>
+      <c r="N11">
+        <v>95.015000000000001</v>
+      </c>
+      <c r="O11">
+        <v>1.879</v>
+      </c>
+      <c r="P11">
+        <v>36.078000000000003</v>
+      </c>
+      <c r="Q11">
+        <v>16.033000000000001</v>
+      </c>
+      <c r="R11">
+        <v>229.053</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="V11">
+        <v>40.201000000000001</v>
+      </c>
+      <c r="W11">
+        <v>13.538</v>
+      </c>
+      <c r="X11">
+        <v>173.25</v>
+      </c>
+      <c r="Y11">
+        <v>360.14600000000002</v>
+      </c>
+      <c r="Z11">
+        <v>16.088999999999999</v>
+      </c>
+      <c r="AA11">
+        <v>87.835999999999999</v>
+      </c>
+      <c r="AB11">
+        <v>11</v>
+      </c>
+      <c r="AC11">
+        <v>3</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AF11">
+        <v>0.35</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>0.99</v>
+      </c>
+      <c r="AI11">
+        <v>0.99</v>
+      </c>
+      <c r="AJ11">
+        <v>12.4</v>
+      </c>
+      <c r="AK11">
+        <v>251.601</v>
+      </c>
+      <c r="AL11">
+        <v>20.29</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12">
+        <v>95.974000000000004</v>
+      </c>
+      <c r="G12">
+        <v>71.78</v>
+      </c>
+      <c r="H12">
+        <v>1380.2650000000001</v>
+      </c>
+      <c r="I12">
+        <v>20.163</v>
+      </c>
+      <c r="J12">
+        <v>403.452</v>
+      </c>
+      <c r="K12">
+        <v>4.0309999999999997</v>
+      </c>
+      <c r="L12">
+        <v>116.087</v>
+      </c>
+      <c r="M12">
+        <v>36.271999999999998</v>
+      </c>
+      <c r="N12">
+        <v>678.95299999999997</v>
+      </c>
+      <c r="O12">
+        <v>27.933</v>
+      </c>
+      <c r="P12">
+        <v>527.79899999999998</v>
+      </c>
+      <c r="Q12">
+        <v>20.513000000000002</v>
+      </c>
+      <c r="R12">
+        <v>317.69400000000002</v>
+      </c>
+      <c r="S12">
+        <v>11.256</v>
+      </c>
+      <c r="T12">
+        <v>375.358</v>
+      </c>
+      <c r="U12">
+        <v>3.6040000000000001</v>
+      </c>
+      <c r="V12">
+        <v>27.462</v>
+      </c>
+      <c r="W12">
+        <v>7.7690000000000001</v>
+      </c>
+      <c r="X12">
+        <v>93.575000000000003</v>
+      </c>
+      <c r="Y12">
+        <v>1899.8040000000001</v>
+      </c>
+      <c r="Z12">
+        <v>19.795000000000002</v>
+      </c>
+      <c r="AA12">
+        <v>20.66</v>
+      </c>
+      <c r="AB12">
+        <v>2</v>
+      </c>
+      <c r="AC12">
+        <v>3</v>
+      </c>
+      <c r="AD12">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AE12">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0.115</v>
+      </c>
+      <c r="AI12">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="AJ12">
+        <v>19.3</v>
+      </c>
+      <c r="AK12">
+        <v>548.221</v>
+      </c>
+      <c r="AL12">
+        <v>28.405000000000001</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13">
+        <v>121.54300000000001</v>
+      </c>
+      <c r="G13">
+        <v>78.02</v>
+      </c>
+      <c r="H13">
+        <v>1435.432</v>
+      </c>
+      <c r="I13">
+        <v>34.542999999999999</v>
+      </c>
+      <c r="J13">
+        <v>773.03599999999994</v>
+      </c>
+      <c r="K13">
+        <v>8.98</v>
+      </c>
+      <c r="L13">
+        <v>226.23599999999999</v>
+      </c>
+      <c r="M13">
+        <v>21.951000000000001</v>
+      </c>
+      <c r="N13">
+        <v>466.70100000000002</v>
+      </c>
+      <c r="O13">
+        <v>28.048999999999999</v>
+      </c>
+      <c r="P13">
+        <v>547.95299999999997</v>
+      </c>
+      <c r="Q13">
+        <v>40.073999999999998</v>
+      </c>
+      <c r="R13">
+        <v>757.44899999999996</v>
+      </c>
+      <c r="S13">
+        <v>31.469000000000001</v>
+      </c>
+      <c r="T13">
+        <v>662.601</v>
+      </c>
+      <c r="U13">
+        <v>3.8</v>
+      </c>
+      <c r="V13">
+        <v>55.061999999999998</v>
+      </c>
+      <c r="W13">
+        <v>9.9410000000000007</v>
+      </c>
+      <c r="X13">
+        <v>162.55699999999999</v>
+      </c>
+      <c r="Y13">
+        <v>2434.7040000000002</v>
+      </c>
+      <c r="Z13">
+        <v>20.032</v>
+      </c>
+      <c r="AA13">
+        <v>94.748999999999995</v>
+      </c>
+      <c r="AB13">
+        <v>4</v>
+      </c>
+      <c r="AC13">
+        <v>5</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AF13">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="AG13">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AH13">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AI13">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="AJ13">
+        <v>41.5</v>
+      </c>
+      <c r="AK13">
+        <v>945.73500000000001</v>
+      </c>
+      <c r="AL13">
+        <v>22.789000000000001</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14">
+        <v>121.54</v>
+      </c>
+      <c r="G14">
+        <v>81.561999999999998</v>
+      </c>
+      <c r="H14">
+        <v>1730.114</v>
+      </c>
+      <c r="I14">
+        <v>29.091000000000001</v>
+      </c>
+      <c r="J14">
+        <v>677.58</v>
+      </c>
+      <c r="K14">
+        <v>10.887</v>
+      </c>
+      <c r="L14">
+        <v>256.83199999999999</v>
+      </c>
+      <c r="M14">
+        <v>51.098999999999997</v>
+      </c>
+      <c r="N14">
+        <v>1074.1199999999999</v>
+      </c>
+      <c r="O14">
+        <v>38.645000000000003</v>
+      </c>
+      <c r="P14">
+        <v>844.96</v>
+      </c>
+      <c r="Q14">
+        <v>16.369</v>
+      </c>
+      <c r="R14">
+        <v>357.392</v>
+      </c>
+      <c r="S14">
+        <v>15.427</v>
+      </c>
+      <c r="T14">
+        <v>388.05500000000001</v>
+      </c>
+      <c r="U14">
+        <v>0.433</v>
+      </c>
+      <c r="V14">
+        <v>7.4039999999999999</v>
+      </c>
+      <c r="W14">
+        <v>5.4720000000000004</v>
+      </c>
+      <c r="X14">
+        <v>116.503</v>
+      </c>
+      <c r="Y14">
+        <v>2664.527</v>
+      </c>
+      <c r="Z14">
+        <v>21.922999999999998</v>
+      </c>
+      <c r="AA14">
+        <v>75.876999999999995</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>7</v>
+      </c>
+      <c r="AD14">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AE14">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AF14">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AG14">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AJ14">
+        <v>109</v>
+      </c>
+      <c r="AK14">
+        <v>2600.8710000000001</v>
+      </c>
+      <c r="AL14">
+        <v>23.861000000000001</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN14" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15">
+        <v>32.76</v>
+      </c>
+      <c r="G15">
+        <v>21.815000000000001</v>
+      </c>
+      <c r="H15">
+        <v>318.32799999999997</v>
+      </c>
+      <c r="I15">
+        <v>9.5410000000000004</v>
+      </c>
+      <c r="J15">
+        <v>125.764</v>
+      </c>
+      <c r="K15">
+        <v>1.4039999999999999</v>
+      </c>
+      <c r="L15">
+        <v>31.061</v>
+      </c>
+      <c r="M15">
+        <v>7.6369999999999996</v>
+      </c>
+      <c r="N15">
+        <v>131.578</v>
+      </c>
+      <c r="O15">
+        <v>10.576000000000001</v>
+      </c>
+      <c r="P15">
+        <v>163.22999999999999</v>
+      </c>
+      <c r="Q15">
+        <v>12.907</v>
+      </c>
+      <c r="R15">
+        <v>136.36799999999999</v>
+      </c>
+      <c r="S15">
+        <v>1.64</v>
+      </c>
+      <c r="T15">
+        <v>43.976999999999997</v>
+      </c>
+      <c r="U15">
+        <v>5.79</v>
+      </c>
+      <c r="V15">
+        <v>35.494999999999997</v>
+      </c>
+      <c r="W15">
+        <v>6.5529999999999999</v>
+      </c>
+      <c r="X15">
+        <v>46.912999999999997</v>
+      </c>
+      <c r="Y15">
+        <v>475.15300000000002</v>
+      </c>
+      <c r="Z15">
+        <v>14.504</v>
+      </c>
+      <c r="AA15">
+        <v>155.773</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0.02</v>
+      </c>
+      <c r="AG15">
+        <v>0.12</v>
+      </c>
+      <c r="AH15">
+        <v>0.02</v>
+      </c>
+      <c r="AI15">
+        <v>0.997</v>
+      </c>
+      <c r="AJ15">
+        <v>15.3</v>
+      </c>
+      <c r="AK15">
+        <v>293.90100000000001</v>
+      </c>
+      <c r="AL15">
+        <v>19.209</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN15" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16">
+        <v>121.553</v>
+      </c>
+      <c r="G16">
+        <v>112.773</v>
+      </c>
+      <c r="H16">
+        <v>1955.9559999999999</v>
+      </c>
+      <c r="I16">
+        <v>6.9850000000000003</v>
+      </c>
+      <c r="J16">
+        <v>148.97499999999999</v>
+      </c>
+      <c r="K16">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="L16">
+        <v>72.858000000000004</v>
+      </c>
+      <c r="M16">
+        <v>42.08</v>
+      </c>
+      <c r="N16">
+        <v>717.35900000000004</v>
+      </c>
+      <c r="O16">
+        <v>30.001999999999999</v>
+      </c>
+      <c r="P16">
+        <v>449.53399999999999</v>
+      </c>
+      <c r="Q16">
+        <v>24.568999999999999</v>
+      </c>
+      <c r="R16">
+        <v>479.12099999999998</v>
+      </c>
+      <c r="S16">
+        <v>24.902000000000001</v>
+      </c>
+      <c r="T16">
+        <v>531.77499999999998</v>
+      </c>
+      <c r="U16">
+        <v>0.224</v>
+      </c>
+      <c r="V16">
+        <v>1.51</v>
+      </c>
+      <c r="W16">
+        <v>1.8740000000000001</v>
+      </c>
+      <c r="X16">
+        <v>51.917000000000002</v>
+      </c>
+      <c r="Y16">
+        <v>2177.788</v>
+      </c>
+      <c r="Z16">
+        <v>17.916</v>
+      </c>
+      <c r="AA16">
+        <v>81.391000000000005</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>2</v>
+      </c>
+      <c r="AD16">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AE16">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AF16">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>28.8</v>
+      </c>
+      <c r="AK16">
+        <v>586.89599999999996</v>
+      </c>
+      <c r="AL16">
+        <v>20.378</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17">
+        <v>43.9</v>
+      </c>
+      <c r="G17">
+        <v>36.908999999999999</v>
+      </c>
+      <c r="H17">
+        <v>708.67899999999997</v>
+      </c>
+      <c r="I17">
+        <v>6.9909999999999997</v>
+      </c>
+      <c r="J17">
+        <v>130.88</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>11.346</v>
+      </c>
+      <c r="N17">
+        <v>256.00700000000001</v>
+      </c>
+      <c r="O17">
+        <v>9.0239999999999991</v>
+      </c>
+      <c r="P17">
+        <v>214.28299999999999</v>
+      </c>
+      <c r="Q17">
+        <v>11.260999999999999</v>
+      </c>
+      <c r="R17">
+        <v>197.74299999999999</v>
+      </c>
+      <c r="S17">
+        <v>12.269</v>
+      </c>
+      <c r="T17">
+        <v>171.52500000000001</v>
+      </c>
+      <c r="U17">
+        <v>3.2730000000000001</v>
+      </c>
+      <c r="V17">
+        <v>7.4429999999999996</v>
+      </c>
+      <c r="W17">
+        <v>3.3820000000000001</v>
+      </c>
+      <c r="X17">
+        <v>17.564</v>
+      </c>
+      <c r="Y17">
+        <v>839.55799999999999</v>
+      </c>
+      <c r="Z17">
+        <v>19.123999999999999</v>
+      </c>
+      <c r="AA17">
+        <v>152.904</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN17" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18">
+        <v>42.807000000000002</v>
+      </c>
+      <c r="G18">
+        <v>28.689</v>
+      </c>
+      <c r="H18">
+        <v>508.22500000000002</v>
+      </c>
+      <c r="I18">
+        <v>11.074999999999999</v>
+      </c>
+      <c r="J18">
+        <v>230.70699999999999</v>
+      </c>
+      <c r="K18">
+        <v>3.0430000000000001</v>
+      </c>
+      <c r="L18">
+        <v>78.908000000000001</v>
+      </c>
+      <c r="M18">
+        <v>5.1230000000000002</v>
+      </c>
+      <c r="N18">
+        <v>95.819000000000003</v>
+      </c>
+      <c r="O18">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="P18">
+        <v>13.659000000000001</v>
+      </c>
+      <c r="Q18">
+        <v>16.594999999999999</v>
+      </c>
+      <c r="R18">
+        <v>317.36900000000003</v>
+      </c>
+      <c r="S18">
+        <v>20.625</v>
+      </c>
+      <c r="T18">
+        <v>390.99299999999999</v>
+      </c>
+      <c r="U18">
+        <v>1.204</v>
+      </c>
+      <c r="V18">
+        <v>9.4909999999999997</v>
+      </c>
+      <c r="W18">
+        <v>4.7160000000000002</v>
+      </c>
+      <c r="X18">
+        <v>57.805999999999997</v>
+      </c>
+      <c r="Y18">
+        <v>817.84</v>
+      </c>
+      <c r="Z18">
+        <v>19.105</v>
+      </c>
+      <c r="AA18">
+        <v>125.851</v>
+      </c>
+      <c r="AB18">
+        <v>5</v>
+      </c>
+      <c r="AC18">
+        <v>3</v>
+      </c>
+      <c r="AD18">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="AJ18">
+        <v>36.5</v>
+      </c>
+      <c r="AK18">
+        <v>794.726</v>
+      </c>
+      <c r="AL18">
+        <v>21.773</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN18" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19">
+        <v>51.216000000000001</v>
+      </c>
+      <c r="G19">
+        <v>39.206000000000003</v>
+      </c>
+      <c r="H19">
+        <v>404.99400000000003</v>
+      </c>
+      <c r="I19">
+        <v>11.901</v>
+      </c>
+      <c r="J19">
+        <v>81.548000000000002</v>
+      </c>
+      <c r="K19">
+        <v>0.109</v>
+      </c>
+      <c r="L19">
+        <v>13.647</v>
+      </c>
+      <c r="M19">
+        <v>18.673999999999999</v>
+      </c>
+      <c r="N19">
+        <v>231.29499999999999</v>
+      </c>
+      <c r="O19">
+        <v>23.695</v>
+      </c>
+      <c r="P19">
+        <v>216.18299999999999</v>
+      </c>
+      <c r="Q19">
+        <v>8.8469999999999995</v>
+      </c>
+      <c r="R19">
+        <v>52.710999999999999</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0.104</v>
+      </c>
+      <c r="V19">
+        <v>0.34</v>
+      </c>
+      <c r="W19">
+        <v>6.883</v>
+      </c>
+      <c r="X19">
+        <v>24.245999999999999</v>
+      </c>
+      <c r="Y19">
+        <v>500.18900000000002</v>
+      </c>
+      <c r="Z19">
+        <v>9.766</v>
+      </c>
+      <c r="AA19">
+        <v>62.555999999999997</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="AJ19">
+        <v>44.2</v>
+      </c>
+      <c r="AK19">
+        <v>492.56</v>
+      </c>
+      <c r="AL19">
+        <v>11.144</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN19" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20">
+        <v>88.986000000000004</v>
+      </c>
+      <c r="G20">
+        <v>75.281000000000006</v>
+      </c>
+      <c r="H20">
+        <v>868.07899999999995</v>
+      </c>
+      <c r="I20">
+        <v>13.705</v>
+      </c>
+      <c r="J20">
+        <v>120.595</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>17.492000000000001</v>
+      </c>
+      <c r="N20">
+        <v>542.68600000000004</v>
+      </c>
+      <c r="O20">
+        <v>40.524999999999999</v>
+      </c>
+      <c r="P20">
+        <v>216.08</v>
+      </c>
+      <c r="Q20">
+        <v>25.634</v>
+      </c>
+      <c r="R20">
+        <v>135.30699999999999</v>
+      </c>
+      <c r="S20">
+        <v>5.335</v>
+      </c>
+      <c r="T20">
+        <v>94.602000000000004</v>
+      </c>
+      <c r="U20">
+        <v>13.504</v>
+      </c>
+      <c r="V20">
+        <v>43.249000000000002</v>
+      </c>
+      <c r="W20">
+        <v>13.504</v>
+      </c>
+      <c r="X20">
+        <v>43.249000000000002</v>
+      </c>
+      <c r="Y20">
+        <v>988.67499999999995</v>
+      </c>
+      <c r="Z20">
+        <v>11.11</v>
+      </c>
+      <c r="AA20">
+        <v>34.463999999999999</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="AJ20">
+        <v>24.7</v>
+      </c>
+      <c r="AK20">
+        <v>371.67500000000001</v>
+      </c>
+      <c r="AL20">
+        <v>15.048</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN20" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21">
+        <v>27.521999999999998</v>
+      </c>
+      <c r="G21">
+        <v>15.531000000000001</v>
+      </c>
+      <c r="H21">
+        <v>252.42400000000001</v>
+      </c>
+      <c r="I21">
+        <v>9.7850000000000001</v>
+      </c>
+      <c r="J21">
+        <v>183.94300000000001</v>
+      </c>
+      <c r="K21">
+        <v>2.206</v>
+      </c>
+      <c r="L21">
+        <v>62.448</v>
+      </c>
+      <c r="M21">
+        <v>3.4969999999999999</v>
+      </c>
+      <c r="N21">
+        <v>67.177000000000007</v>
+      </c>
+      <c r="O21">
+        <v>6.66</v>
+      </c>
+      <c r="P21">
+        <v>121.376</v>
+      </c>
+      <c r="Q21">
+        <v>15.176</v>
+      </c>
+      <c r="R21">
+        <v>258.61500000000001</v>
+      </c>
+      <c r="S21">
+        <v>2.1890000000000001</v>
+      </c>
+      <c r="T21">
+        <v>51.646000000000001</v>
+      </c>
+      <c r="U21">
+        <v>2.4830000000000001</v>
+      </c>
+      <c r="V21">
+        <v>21.151</v>
+      </c>
+      <c r="W21">
+        <v>6.4409999999999998</v>
+      </c>
+      <c r="X21">
+        <v>97.234999999999999</v>
+      </c>
+      <c r="Y21">
+        <v>498.815</v>
+      </c>
+      <c r="Z21">
+        <v>18.123999999999999</v>
+      </c>
+      <c r="AA21">
+        <v>103.99299999999999</v>
+      </c>
+      <c r="AB21">
+        <v>4</v>
+      </c>
+      <c r="AC21">
+        <v>4</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AF21">
+        <v>0.19</v>
+      </c>
+      <c r="AG21">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="AH21">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AI21">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="AJ21">
+        <v>23.9</v>
+      </c>
+      <c r="AK21">
+        <v>486.50900000000001</v>
+      </c>
+      <c r="AL21">
+        <v>20.356000000000002</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN21" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22">
+        <v>121.56100000000001</v>
+      </c>
+      <c r="G22">
+        <v>80.581999999999994</v>
+      </c>
+      <c r="H22">
+        <v>1583.201</v>
+      </c>
+      <c r="I22">
+        <v>33.338000000000001</v>
+      </c>
+      <c r="J22">
+        <v>800.18399999999997</v>
+      </c>
+      <c r="K22">
+        <v>7.641</v>
+      </c>
+      <c r="L22">
+        <v>143.63900000000001</v>
+      </c>
+      <c r="M22">
+        <v>31.823</v>
+      </c>
+      <c r="N22">
+        <v>697.23599999999999</v>
+      </c>
+      <c r="O22">
+        <v>29.504000000000001</v>
+      </c>
+      <c r="P22">
+        <v>557.70799999999997</v>
+      </c>
+      <c r="Q22">
+        <v>29.030999999999999</v>
+      </c>
+      <c r="R22">
+        <v>606.13199999999995</v>
+      </c>
+      <c r="S22">
+        <v>31.202999999999999</v>
+      </c>
+      <c r="T22">
+        <v>665.94799999999998</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>7.4249999999999998</v>
+      </c>
+      <c r="X22">
+        <v>142.93299999999999</v>
+      </c>
+      <c r="Y22">
+        <v>2527.0239999999999</v>
+      </c>
+      <c r="Z22">
+        <v>20.788</v>
+      </c>
+      <c r="AA22">
+        <v>41.082999999999998</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>10</v>
+      </c>
+      <c r="AD22">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AE22">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AH22">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AI22">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN22" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23">
+        <v>121.538</v>
+      </c>
+      <c r="G23">
+        <v>119.355</v>
+      </c>
+      <c r="H23">
+        <v>2300.201</v>
+      </c>
+      <c r="I23">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="J23">
+        <v>31.863</v>
+      </c>
+      <c r="K23">
+        <v>0.87</v>
+      </c>
+      <c r="L23">
+        <v>24.983000000000001</v>
+      </c>
+      <c r="M23">
+        <v>31.102</v>
+      </c>
+      <c r="N23">
+        <v>534.60500000000002</v>
+      </c>
+      <c r="O23">
+        <v>35.54</v>
+      </c>
+      <c r="P23">
+        <v>671.23299999999995</v>
+      </c>
+      <c r="Q23">
+        <v>31.300999999999998</v>
+      </c>
+      <c r="R23">
+        <v>635.11300000000006</v>
+      </c>
+      <c r="S23">
+        <v>23.594999999999999</v>
+      </c>
+      <c r="T23">
+        <v>516.09500000000003</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="X23">
+        <v>30.902999999999999</v>
+      </c>
+      <c r="Y23">
+        <v>2357.047</v>
+      </c>
+      <c r="Z23">
+        <v>19.393000000000001</v>
+      </c>
+      <c r="AA23">
+        <v>43.493000000000002</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>2</v>
+      </c>
+      <c r="AD23">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24">
+        <v>27.626999999999999</v>
+      </c>
+      <c r="G24">
+        <v>15.398999999999999</v>
+      </c>
+      <c r="H24">
+        <v>416.19600000000003</v>
+      </c>
+      <c r="I24">
+        <v>11.57</v>
+      </c>
+      <c r="J24">
+        <v>185.66900000000001</v>
+      </c>
+      <c r="K24">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="L24">
+        <v>19.192</v>
+      </c>
+      <c r="M24">
+        <v>5.8959999999999999</v>
+      </c>
+      <c r="N24">
+        <v>155.99299999999999</v>
+      </c>
+      <c r="O24">
+        <v>6.7930000000000001</v>
+      </c>
+      <c r="P24">
+        <v>181.57400000000001</v>
+      </c>
+      <c r="Q24">
+        <v>10.57</v>
+      </c>
+      <c r="R24">
+        <v>159.09299999999999</v>
+      </c>
+      <c r="S24">
+        <v>4.3680000000000003</v>
+      </c>
+      <c r="T24">
+        <v>124.39700000000001</v>
+      </c>
+      <c r="U24">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="V24">
+        <v>6.95</v>
+      </c>
+      <c r="W24">
+        <v>6.3209999999999997</v>
+      </c>
+      <c r="X24">
+        <v>44.534999999999997</v>
+      </c>
+      <c r="Y24">
+        <v>621.05700000000002</v>
+      </c>
+      <c r="Z24">
+        <v>22.48</v>
+      </c>
+      <c r="AA24">
+        <v>76.965999999999994</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
+        <v>2</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>9.4E-2</v>
+      </c>
+      <c r="AG24">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AH24">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AI24">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="AJ24">
+        <v>23.8</v>
+      </c>
+      <c r="AK24">
+        <v>617.19399999999996</v>
+      </c>
+      <c r="AL24">
+        <v>25.933</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN24" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25">
+        <v>56.57</v>
+      </c>
+      <c r="G25">
+        <v>38.978000000000002</v>
+      </c>
+      <c r="H25">
+        <v>660.58100000000002</v>
+      </c>
+      <c r="I25">
+        <v>13.234999999999999</v>
+      </c>
+      <c r="J25">
+        <v>283.142</v>
+      </c>
+      <c r="K25">
+        <v>4.3570000000000002</v>
+      </c>
+      <c r="L25">
+        <v>102.559</v>
+      </c>
+      <c r="M25">
+        <v>19.885999999999999</v>
+      </c>
+      <c r="N25">
+        <v>384.76100000000002</v>
+      </c>
+      <c r="O25">
+        <v>20.417999999999999</v>
+      </c>
+      <c r="P25">
+        <v>341.47899999999998</v>
+      </c>
+      <c r="Q25">
+        <v>7.3159999999999998</v>
+      </c>
+      <c r="R25">
+        <v>132.375</v>
+      </c>
+      <c r="S25">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="T25">
+        <v>187.667</v>
+      </c>
+      <c r="U25">
+        <v>3.1619999999999999</v>
+      </c>
+      <c r="V25">
+        <v>30.204999999999998</v>
+      </c>
+      <c r="W25">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="X25">
+        <v>45.515999999999998</v>
+      </c>
+      <c r="Y25">
+        <v>1046.2829999999999</v>
+      </c>
+      <c r="Z25">
+        <v>18.495000000000001</v>
+      </c>
+      <c r="AA25">
+        <v>30.812999999999999</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>2.3E-2</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <v>0</v>
+      </c>
+      <c r="AH25">
+        <v>0</v>
+      </c>
+      <c r="AI25">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="AJ25">
+        <v>49.1</v>
+      </c>
+      <c r="AK25">
+        <v>1018.801</v>
+      </c>
+      <c r="AL25">
+        <v>20.75</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN25" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26">
+        <v>59.405999999999999</v>
+      </c>
+      <c r="G26">
+        <v>42.459000000000003</v>
+      </c>
+      <c r="H26">
+        <v>568.68600000000004</v>
+      </c>
+      <c r="I26">
+        <v>13.035</v>
+      </c>
+      <c r="J26">
+        <v>197.93700000000001</v>
+      </c>
+      <c r="K26">
+        <v>3.9119999999999999</v>
+      </c>
+      <c r="L26">
+        <v>56.481999999999999</v>
+      </c>
+      <c r="M26">
+        <v>14.88</v>
+      </c>
+      <c r="N26">
+        <v>192.465</v>
+      </c>
+      <c r="O26">
+        <v>29.053999999999998</v>
+      </c>
+      <c r="P26">
+        <v>419.63099999999997</v>
+      </c>
+      <c r="Q26">
+        <v>15.472</v>
+      </c>
+      <c r="R26">
+        <v>211.00899999999999</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>3.052</v>
+      </c>
+      <c r="V26">
+        <v>22.628</v>
+      </c>
+      <c r="W26">
+        <v>5.218</v>
+      </c>
+      <c r="X26">
+        <v>60.91</v>
+      </c>
+      <c r="Y26">
+        <v>823.10500000000002</v>
+      </c>
+      <c r="Z26">
+        <v>13.856</v>
+      </c>
+      <c r="AA26">
+        <v>119.64</v>
+      </c>
+      <c r="AB26">
+        <v>2</v>
+      </c>
+      <c r="AC26">
+        <v>2</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="AH26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="AJ26">
+        <v>51.8</v>
+      </c>
+      <c r="AK26">
+        <v>800.97</v>
+      </c>
+      <c r="AL26">
+        <v>15.462999999999999</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN26" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27">
+        <v>19.986000000000001</v>
+      </c>
+      <c r="G27">
+        <v>10.545999999999999</v>
+      </c>
+      <c r="H27">
+        <v>255.90600000000001</v>
+      </c>
+      <c r="I27">
+        <v>8.2149999999999999</v>
+      </c>
+      <c r="J27">
+        <v>138.995</v>
+      </c>
+      <c r="K27">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="L27">
+        <v>52.075000000000003</v>
+      </c>
+      <c r="M27">
+        <v>5.452</v>
+      </c>
+      <c r="N27">
+        <v>136.15</v>
+      </c>
+      <c r="O27">
+        <v>3.194</v>
+      </c>
+      <c r="P27">
+        <v>68.602000000000004</v>
+      </c>
+      <c r="Q27">
+        <v>6.11</v>
+      </c>
+      <c r="R27">
+        <v>75.150000000000006</v>
+      </c>
+      <c r="S27">
+        <v>5.23</v>
+      </c>
+      <c r="T27">
+        <v>167.07300000000001</v>
+      </c>
+      <c r="U27">
+        <v>3.274</v>
+      </c>
+      <c r="V27">
+        <v>8.2590000000000003</v>
+      </c>
+      <c r="W27">
+        <v>3.492</v>
+      </c>
+      <c r="X27">
+        <v>12.507999999999999</v>
+      </c>
+      <c r="Y27">
+        <v>446.976</v>
+      </c>
+      <c r="Z27">
+        <v>22.364000000000001</v>
+      </c>
+      <c r="AA27">
+        <v>94.625</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="AI27">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN27" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28">
+        <v>41.499000000000002</v>
+      </c>
+      <c r="G28">
+        <v>17.256</v>
+      </c>
+      <c r="H28">
+        <v>313.721</v>
+      </c>
+      <c r="I28">
+        <v>18.701000000000001</v>
+      </c>
+      <c r="J28">
+        <v>356.21499999999997</v>
+      </c>
+      <c r="K28">
+        <v>5.5419999999999998</v>
+      </c>
+      <c r="L28">
+        <v>118.392</v>
+      </c>
+      <c r="M28">
+        <v>10.164999999999999</v>
+      </c>
+      <c r="N28">
+        <v>215.23400000000001</v>
+      </c>
+      <c r="O28">
+        <v>6.2210000000000001</v>
+      </c>
+      <c r="P28">
+        <v>142.126</v>
+      </c>
+      <c r="Q28">
+        <v>15.827</v>
+      </c>
+      <c r="R28">
+        <v>236.339</v>
+      </c>
+      <c r="S28">
+        <v>9.2859999999999996</v>
+      </c>
+      <c r="T28">
+        <v>194.63</v>
+      </c>
+      <c r="U28">
+        <v>4.4770000000000003</v>
+      </c>
+      <c r="V28">
+        <v>50.755000000000003</v>
+      </c>
+      <c r="W28">
+        <v>10.253</v>
+      </c>
+      <c r="X28">
+        <v>142.39400000000001</v>
+      </c>
+      <c r="Y28">
+        <v>788.32799999999997</v>
+      </c>
+      <c r="Z28">
+        <v>18.995999999999999</v>
+      </c>
+      <c r="AA28">
+        <v>16.381</v>
+      </c>
+      <c r="AB28">
+        <v>13</v>
+      </c>
+      <c r="AC28">
+        <v>2</v>
+      </c>
+      <c r="AD28">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="AE28">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AF28">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AG28">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="AH28">
+        <v>0</v>
+      </c>
+      <c r="AI28">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="AJ28">
+        <v>12.3</v>
+      </c>
+      <c r="AK28">
+        <v>301.07600000000002</v>
+      </c>
+      <c r="AL28">
+        <v>24.478000000000002</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN28" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29">
+        <v>121.541</v>
+      </c>
+      <c r="G29">
+        <v>83.218999999999994</v>
+      </c>
+      <c r="H29">
+        <v>1891.9829999999999</v>
+      </c>
+      <c r="I29">
+        <v>29.376000000000001</v>
+      </c>
+      <c r="J29">
+        <v>703</v>
+      </c>
+      <c r="K29">
+        <v>8.9459999999999997</v>
+      </c>
+      <c r="L29">
+        <v>218.154</v>
+      </c>
+      <c r="M29">
+        <v>39.409999999999997</v>
+      </c>
+      <c r="N29">
+        <v>948.93100000000004</v>
+      </c>
+      <c r="O29">
+        <v>26.015999999999998</v>
+      </c>
+      <c r="P29">
+        <v>587.17100000000005</v>
+      </c>
+      <c r="Q29">
+        <v>20.84</v>
+      </c>
+      <c r="R29">
+        <v>429.637</v>
+      </c>
+      <c r="S29">
+        <v>35.274999999999999</v>
+      </c>
+      <c r="T29">
+        <v>847.39800000000002</v>
+      </c>
+      <c r="U29">
+        <v>1.089</v>
+      </c>
+      <c r="V29">
+        <v>16.331</v>
+      </c>
+      <c r="W29">
+        <v>7.0119999999999996</v>
+      </c>
+      <c r="X29">
+        <v>122.96</v>
+      </c>
+      <c r="Y29">
+        <v>2813.1370000000002</v>
+      </c>
+      <c r="Z29">
+        <v>23.146000000000001</v>
+      </c>
+      <c r="AA29">
+        <v>67.501999999999995</v>
+      </c>
+      <c r="AB29">
+        <v>0</v>
+      </c>
+      <c r="AC29">
+        <v>6</v>
+      </c>
+      <c r="AD29">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AE29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AG29">
+        <v>0</v>
+      </c>
+      <c r="AH29">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AI29">
+        <v>0.151</v>
+      </c>
+      <c r="AJ29">
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <v>0</v>
+      </c>
+      <c r="AL29">
+        <v>0</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN29" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30">
+        <v>121.54</v>
+      </c>
+      <c r="G30">
+        <v>117.511</v>
+      </c>
+      <c r="H30">
+        <v>1892.164</v>
+      </c>
+      <c r="I30">
+        <v>4.0289999999999999</v>
+      </c>
+      <c r="J30">
+        <v>107.229</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>37.902000000000001</v>
+      </c>
+      <c r="N30">
+        <v>525.73099999999999</v>
+      </c>
+      <c r="O30">
+        <v>38.878</v>
+      </c>
+      <c r="P30">
+        <v>545.49300000000005</v>
+      </c>
+      <c r="Q30">
+        <v>22.053999999999998</v>
+      </c>
+      <c r="R30">
+        <v>465.60500000000002</v>
+      </c>
+      <c r="S30">
+        <v>22.706</v>
+      </c>
+      <c r="T30">
+        <v>462.56299999999999</v>
+      </c>
+      <c r="U30">
+        <v>0.442</v>
+      </c>
+      <c r="V30">
+        <v>15.132</v>
+      </c>
+      <c r="W30">
+        <v>2.411</v>
+      </c>
+      <c r="X30">
+        <v>70.367000000000004</v>
+      </c>
+      <c r="Y30">
+        <v>1999.393</v>
+      </c>
+      <c r="Z30">
+        <v>16.45</v>
+      </c>
+      <c r="AA30">
+        <v>130.11099999999999</v>
+      </c>
+      <c r="AB30">
+        <v>2</v>
+      </c>
+      <c r="AC30">
+        <v>2</v>
+      </c>
+      <c r="AD30">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AE30">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
+      </c>
+      <c r="AG30">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AH30">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="AK30">
+        <v>691.77599999999995</v>
+      </c>
+      <c r="AL30">
+        <v>19.323</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31">
+        <v>121.557</v>
+      </c>
+      <c r="G31">
+        <v>97.763999999999996</v>
+      </c>
+      <c r="H31">
+        <v>2095.5349999999999</v>
+      </c>
+      <c r="I31">
+        <v>20.846</v>
+      </c>
+      <c r="J31">
+        <v>522.57799999999997</v>
+      </c>
+      <c r="K31">
+        <v>2.9470000000000001</v>
+      </c>
+      <c r="L31">
+        <v>74.790999999999997</v>
+      </c>
+      <c r="M31">
+        <v>29.31</v>
+      </c>
+      <c r="N31">
+        <v>613.39599999999996</v>
+      </c>
+      <c r="O31">
+        <v>28.274999999999999</v>
+      </c>
+      <c r="P31">
+        <v>586.54700000000003</v>
+      </c>
+      <c r="Q31">
+        <v>34.573999999999998</v>
+      </c>
+      <c r="R31">
+        <v>794.83299999999997</v>
+      </c>
+      <c r="S31">
+        <v>29.398</v>
+      </c>
+      <c r="T31">
+        <v>698.12800000000004</v>
+      </c>
+      <c r="U31">
+        <v>1.087</v>
+      </c>
+      <c r="V31">
+        <v>28.209</v>
+      </c>
+      <c r="W31">
+        <v>4.4420000000000002</v>
+      </c>
+      <c r="X31">
+        <v>120.096</v>
+      </c>
+      <c r="Y31">
+        <v>2692.904</v>
+      </c>
+      <c r="Z31">
+        <v>22.152999999999999</v>
+      </c>
+      <c r="AA31">
+        <v>45.651000000000003</v>
+      </c>
+      <c r="AB31">
+        <v>3</v>
+      </c>
+      <c r="AC31">
+        <v>5</v>
+      </c>
+      <c r="AD31">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AE31">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AF31">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AG31">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AH31">
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>19</v>
+      </c>
+      <c r="AK31">
+        <v>556.57799999999997</v>
+      </c>
+      <c r="AL31">
+        <v>29.294</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN31" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32">
+        <v>121.54600000000001</v>
+      </c>
+      <c r="G32">
+        <v>104.32899999999999</v>
+      </c>
+      <c r="H32">
+        <v>1586.4380000000001</v>
+      </c>
+      <c r="I32">
+        <v>12.417999999999999</v>
+      </c>
+      <c r="J32">
+        <v>323.57600000000002</v>
+      </c>
+      <c r="K32">
+        <v>4.7990000000000004</v>
+      </c>
+      <c r="L32">
+        <v>103.791</v>
+      </c>
+      <c r="M32">
+        <v>17.611000000000001</v>
+      </c>
+      <c r="N32">
+        <v>303.74799999999999</v>
+      </c>
+      <c r="O32">
+        <v>17.373999999999999</v>
+      </c>
+      <c r="P32">
+        <v>337.47800000000001</v>
+      </c>
+      <c r="Q32">
+        <v>62.018000000000001</v>
+      </c>
+      <c r="R32">
+        <v>898.53700000000003</v>
+      </c>
+      <c r="S32">
+        <v>24.542999999999999</v>
+      </c>
+      <c r="T32">
+        <v>474.041</v>
+      </c>
+      <c r="U32">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="V32">
+        <v>7.7350000000000003</v>
+      </c>
+      <c r="W32">
+        <v>2.9369999999999998</v>
+      </c>
+      <c r="X32">
+        <v>67.558999999999997</v>
+      </c>
+      <c r="Y32">
+        <v>2013.8050000000001</v>
+      </c>
+      <c r="Z32">
+        <v>16.568000000000001</v>
+      </c>
+      <c r="AA32">
+        <v>59.085999999999999</v>
+      </c>
+      <c r="AB32">
+        <v>1</v>
+      </c>
+      <c r="AC32">
+        <v>4</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="AF32">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AG32">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AH32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AJ32">
+        <v>47.2</v>
+      </c>
+      <c r="AK32">
+        <v>860.34100000000001</v>
+      </c>
+      <c r="AL32">
+        <v>18.228000000000002</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN32" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33">
+        <v>121.544</v>
+      </c>
+      <c r="G33">
+        <v>97.328000000000003</v>
+      </c>
+      <c r="H33">
+        <v>1740.107</v>
+      </c>
+      <c r="I33">
+        <v>20.608000000000001</v>
+      </c>
+      <c r="J33">
+        <v>399.19299999999998</v>
+      </c>
+      <c r="K33">
+        <v>3.6080000000000001</v>
+      </c>
+      <c r="L33">
+        <v>84.971000000000004</v>
+      </c>
+      <c r="M33">
+        <v>9.0449999999999999</v>
+      </c>
+      <c r="N33">
+        <v>168.58500000000001</v>
+      </c>
+      <c r="O33">
+        <v>73.698999999999998</v>
+      </c>
+      <c r="P33">
+        <v>1304.7059999999999</v>
+      </c>
+      <c r="Q33">
+        <v>21.414000000000001</v>
+      </c>
+      <c r="R33">
+        <v>478.988</v>
+      </c>
+      <c r="S33">
+        <v>17.385999999999999</v>
+      </c>
+      <c r="T33">
+        <v>271.99299999999999</v>
+      </c>
+      <c r="U33">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="V33">
+        <v>20.821000000000002</v>
+      </c>
+      <c r="W33">
+        <v>3.3849999999999998</v>
+      </c>
+      <c r="X33">
+        <v>75.852000000000004</v>
+      </c>
+      <c r="Y33">
+        <v>2224.2719999999999</v>
+      </c>
+      <c r="Z33">
+        <v>18.3</v>
+      </c>
+      <c r="AA33">
+        <v>127.32299999999999</v>
+      </c>
+      <c r="AB33">
+        <v>3</v>
+      </c>
+      <c r="AC33">
+        <v>3</v>
+      </c>
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AE33">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AF33">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AI33">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AJ33">
+        <v>33.4</v>
+      </c>
+      <c r="AK33">
+        <v>553.35199999999998</v>
+      </c>
+      <c r="AL33">
+        <v>16.567</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN33" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34">
+        <v>121.538</v>
+      </c>
+      <c r="G34">
+        <v>86.171000000000006</v>
+      </c>
+      <c r="H34">
+        <v>1552.961</v>
+      </c>
+      <c r="I34">
+        <v>29.573</v>
+      </c>
+      <c r="J34">
+        <v>606.63199999999995</v>
+      </c>
+      <c r="K34">
+        <v>5.7939999999999996</v>
+      </c>
+      <c r="L34">
+        <v>168.10900000000001</v>
+      </c>
+      <c r="M34">
+        <v>34.015000000000001</v>
+      </c>
+      <c r="N34">
+        <v>690.29</v>
+      </c>
+      <c r="O34">
+        <v>31.648</v>
+      </c>
+      <c r="P34">
+        <v>598.84100000000001</v>
+      </c>
+      <c r="Q34">
+        <v>29.786000000000001</v>
+      </c>
+      <c r="R34">
+        <v>563.52800000000002</v>
+      </c>
+      <c r="S34">
+        <v>26.088999999999999</v>
+      </c>
+      <c r="T34">
+        <v>475.04300000000001</v>
+      </c>
+      <c r="U34">
+        <v>1.399</v>
+      </c>
+      <c r="V34">
+        <v>34.543999999999997</v>
+      </c>
+      <c r="W34">
+        <v>5.7649999999999997</v>
+      </c>
+      <c r="X34">
+        <v>119.98</v>
+      </c>
+      <c r="Y34">
+        <v>2327.7020000000002</v>
+      </c>
+      <c r="Z34">
+        <v>19.152000000000001</v>
+      </c>
+      <c r="AA34">
+        <v>127.979</v>
+      </c>
+      <c r="AB34">
+        <v>4</v>
+      </c>
+      <c r="AC34">
+        <v>4</v>
+      </c>
+      <c r="AD34">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AE34">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AF34">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AG34">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AH34">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AI34">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AJ34">
+        <v>8.9</v>
+      </c>
+      <c r="AK34">
+        <v>227.53200000000001</v>
+      </c>
+      <c r="AL34">
+        <v>25.565000000000001</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN34" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="AO34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35">
+        <v>121.547</v>
+      </c>
+      <c r="G35">
+        <v>77.885999999999996</v>
+      </c>
+      <c r="H35">
+        <v>1615.6569999999999</v>
+      </c>
+      <c r="I35">
+        <v>35.356999999999999</v>
+      </c>
+      <c r="J35">
+        <v>813.33199999999999</v>
+      </c>
+      <c r="K35">
+        <v>8.3040000000000003</v>
+      </c>
+      <c r="L35">
+        <v>198.709</v>
+      </c>
+      <c r="M35">
+        <v>33.231000000000002</v>
+      </c>
+      <c r="N35">
+        <v>706.87300000000005</v>
+      </c>
+      <c r="O35">
+        <v>26.158000000000001</v>
+      </c>
+      <c r="P35">
+        <v>537.94399999999996</v>
+      </c>
+      <c r="Q35">
+        <v>26.785</v>
+      </c>
+      <c r="R35">
+        <v>605.27800000000002</v>
+      </c>
+      <c r="S35">
+        <v>35.372999999999998</v>
+      </c>
+      <c r="T35">
+        <v>777.60299999999995</v>
+      </c>
+      <c r="U35">
+        <v>2.605</v>
+      </c>
+      <c r="V35">
+        <v>60.933999999999997</v>
+      </c>
+      <c r="W35">
+        <v>8.2759999999999998</v>
+      </c>
+      <c r="X35">
+        <v>196.624</v>
+      </c>
+      <c r="Y35">
+        <v>2627.6979999999999</v>
+      </c>
+      <c r="Z35">
+        <v>21.619</v>
+      </c>
+      <c r="AA35">
+        <v>82.094999999999999</v>
+      </c>
+      <c r="AB35">
+        <v>7</v>
+      </c>
+      <c r="AC35">
+        <v>3</v>
+      </c>
+      <c r="AD35">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AE35">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AF35">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AG35">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AH35">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AI35">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AJ35">
+        <v>22.5</v>
+      </c>
+      <c r="AK35">
+        <v>588.77800000000002</v>
+      </c>
+      <c r="AL35">
+        <v>26.167999999999999</v>
+      </c>
+      <c r="AM35" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN35" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36">
+        <v>121.542</v>
+      </c>
+      <c r="G36">
+        <v>73.313000000000002</v>
+      </c>
+      <c r="H36">
+        <v>1590.1489999999999</v>
+      </c>
+      <c r="I36">
+        <v>38.145000000000003</v>
+      </c>
+      <c r="J36">
+        <v>886.89700000000005</v>
+      </c>
+      <c r="K36">
+        <v>10.084</v>
+      </c>
+      <c r="L36">
+        <v>244.43100000000001</v>
+      </c>
+      <c r="M36">
+        <v>25.802</v>
+      </c>
+      <c r="N36">
+        <v>585.577</v>
+      </c>
+      <c r="O36">
+        <v>20.09</v>
+      </c>
+      <c r="P36">
+        <v>423.98500000000001</v>
+      </c>
+      <c r="Q36">
+        <v>36.256999999999998</v>
+      </c>
+      <c r="R36">
+        <v>775.25599999999997</v>
+      </c>
+      <c r="S36">
+        <v>39.393000000000001</v>
+      </c>
+      <c r="T36">
+        <v>936.65899999999999</v>
+      </c>
+      <c r="U36">
+        <v>1.6419999999999999</v>
+      </c>
+      <c r="V36">
+        <v>39.186</v>
+      </c>
+      <c r="W36">
+        <v>7.734</v>
+      </c>
+      <c r="X36">
+        <v>171.77600000000001</v>
+      </c>
+      <c r="Y36">
+        <v>2721.4769999999999</v>
+      </c>
+      <c r="Z36">
+        <v>22.390999999999998</v>
+      </c>
+      <c r="AA36">
+        <v>146.048</v>
+      </c>
+      <c r="AB36">
+        <v>4</v>
+      </c>
+      <c r="AC36">
+        <v>6</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AF36">
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AH36">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AI36">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AJ36">
+        <v>30</v>
+      </c>
+      <c r="AK36">
+        <v>761.53200000000004</v>
+      </c>
+      <c r="AL36">
+        <v>25.384</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN36" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AO36">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>